<commit_message>
Workaround for exhibition with rotations, contd.
</commit_message>
<xml_diff>
--- a/data/exhibition-scrolls-v2.xlsx
+++ b/data/exhibition-scrolls-v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr updateLinks="always" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hildad/Documents/GitHub/lyingpendatabases/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ludvi\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6033D2-4F08-B444-BFBE-946DBC75AF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED90D88-461E-476C-9EF9-57A31D5F3B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSS Exhibited" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="298">
   <si>
     <t>Exhibitions</t>
   </si>
@@ -1631,6 +1631,12 @@
   </si>
   <si>
     <t>Words from Genesis 22; [ID] 4Q226 psJubb frag. 6a "Genesis Midrash"</t>
+  </si>
+  <si>
+    <t>Artefacts</t>
+  </si>
+  <si>
+    <t>No scrolls</t>
   </si>
 </sst>
 </file>
@@ -2007,7 +2013,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2071,9 +2077,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2179,23 +2182,47 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="6"/>
+        <color theme="0"/>
+        <name val="Aleo Light"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2228,39 +2255,6 @@
         </top>
         <bottom style="thin">
           <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="6"/>
-        <color theme="0"/>
-        <name val="Aleo Light"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
         </bottom>
       </border>
     </dxf>
@@ -2424,14 +2418,11 @@
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
     <sheetNames>
-      <sheetName val="DSS Exhibitions"/>
+      <sheetName val="exhibition-v2"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2447,10 +2438,10 @@
     <tableColumn id="1" xr3:uid="{50F95EDE-B0D4-4E10-9A95-1364B308712E}" name="Group" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{B8B9B968-29C9-4543-9412-E7163369F867}" name="Manuscript" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{ED87D8D3-A856-44E5-A022-A6F75D7EA7A2}" name="Manuscript Content" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{5FC03F6E-2873-485E-A06B-53FACF9E9B49}" name="Exhibitions" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{5FC03F6E-2873-485E-A06B-53FACF9E9B49}" name="Exhibitions" dataDxfId="1">
       <calculatedColumnFormula>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{088EC224-45C3-4867-9B11-C4E28CF74E00}" name="_" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{088EC224-45C3-4867-9B11-C4E28CF74E00}" name="_" dataDxfId="0">
       <calculatedColumnFormula array="1">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</calculatedColumnFormula>
     </tableColumn>
@@ -2460,7 +2451,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2762,21 +2753,21 @@
   <dimension ref="A1:F211"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E159" sqref="E159"/>
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A205" sqref="A205"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="53" customWidth="1"/>
-    <col min="5" max="5" width="65.1640625" style="50" customWidth="1"/>
-    <col min="6" max="6" width="40.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="52" customWidth="1"/>
+    <col min="5" max="5" width="65.140625" style="49" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17.25" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>185</v>
       </c>
@@ -2786,27 +2777,27 @@
       <c r="C1" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="53" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="F1" s="47"/>
-    </row>
-    <row r="2" spans="1:6" ht="135" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="F1" s="46"/>
+    </row>
+    <row r="2" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="C2" s="37"/>
+      <c r="C2" s="36"/>
       <c r="D2" s="13">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>8</v>
       </c>
-      <c r="E2" s="55" t="str" cm="1">
+      <c r="E2" s="54" t="str" cm="1">
         <f t="array" ref="E2">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2009/6/27–2009/10/9: Dead Sea Scrolls: Words that Changed the World at the Royal Ontario Museum
@@ -2818,21 +2809,21 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F2" s="48"/>
-    </row>
-    <row r="3" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="F2" s="47"/>
+    </row>
+    <row r="3" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
         <v>236</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="39">
+      <c r="C3" s="35"/>
+      <c r="D3" s="38">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>8</v>
       </c>
-      <c r="E3" s="56" t="str" cm="1">
+      <c r="E3" s="55" t="str" cm="1">
         <f t="array" ref="E3">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2009/6/27–2010/1/3: Dead Sea Scrolls: Words that Changed the World at the Royal Ontario Museum
@@ -2844,51 +2835,51 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F3" s="48"/>
-    </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="F3" s="47"/>
+    </row>
+    <row r="4" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="40">
+      <c r="C4" s="35"/>
+      <c r="D4" s="39">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E4" s="56" t="str" cm="1">
+      <c r="E4" s="55" t="str" cm="1">
         <f t="array" ref="E4">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1951/1/1–2009/1/1: Exhibition at the Jordan Archaeological Museum
 1964/4/22–1964/10/18: Exhibition at the New York World's Fair
 1965/4/21–1965/10/17: Exhibition at the New York World's Fair</v>
       </c>
-      <c r="F4" s="48"/>
-    </row>
-    <row r="5" spans="1:6" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="32" t="s">
+      <c r="F4" s="47"/>
+    </row>
+    <row r="5" spans="1:6" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>183</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="58">
+      <c r="D5" s="57">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E5" s="56" t="str" cm="1">
+      <c r="E5" s="55" t="str" cm="1">
         <f t="array" ref="E5">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1951/1/1–2009/1/1: Exhibition at the Jordan Archaeological Museum
 1964/4/26–1964/5/10: The Book and the Spade at the Wisconsin Center
 1964/5/21–1964/6/7: The Book and the Spade at the Public Museum of Milwaukee</v>
       </c>
-      <c r="F5" s="48"/>
-    </row>
-    <row r="6" spans="1:6" ht="111" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F5" s="47"/>
+    </row>
+    <row r="6" spans="1:6" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2902,7 +2893,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>4</v>
       </c>
-      <c r="E6" s="56" t="str" cm="1">
+      <c r="E6" s="55" t="str" cm="1">
         <f t="array" ref="E6">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1950/11/17–1950/11/26: Exhibition at the University of Chicago Oriental Institute
@@ -2910,9 +2901,9 @@
 1957/1/1–1957/1/1: Exhibition at the Hebrew University
 1965/4/20–1900/1/0: Exhibition at the Shrine of the Book</v>
       </c>
-      <c r="F6" s="48"/>
-    </row>
-    <row r="7" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F6" s="47"/>
+    </row>
+    <row r="7" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -2924,15 +2915,15 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E7" s="56" t="str" cm="1">
+      <c r="E7" s="55" t="str" cm="1">
         <f t="array" ref="E7">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1950/1/10–1950/1/10: Exhibition at the Zion Research Library
 1950/11/17–1950/11/26: Exhibition at the University of Chicago Oriental Institute</v>
       </c>
-      <c r="F7" s="48"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="47"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
@@ -2944,14 +2935,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E8" s="56" t="str" cm="1">
+      <c r="E8" s="55" t="str" cm="1">
         <f t="array" ref="E8">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1957/3/25–1957/7/21: Exhibition at the Beirut Museum</v>
       </c>
-      <c r="F8" s="48"/>
-    </row>
-    <row r="9" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F8" s="47"/>
+    </row>
+    <row r="9" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -2963,15 +2954,15 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E9" s="56" t="str" cm="1">
+      <c r="E9" s="55" t="str" cm="1">
         <f t="array" ref="E9">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1957/3/25–1957/7/21: Exhibition at the Beirut Museum
 1997/9/1–1997/9/18: Ancient Scrolls from the Dead Sea at the Brigham Young University Museum of Art</v>
       </c>
-      <c r="F9" s="48"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F9" s="47"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>2</v>
       </c>
@@ -2983,14 +2974,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E10" s="56" t="str" cm="1">
+      <c r="E10" s="55" t="str" cm="1">
         <f t="array" ref="E10">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1957/3/25–1957/7/21: Exhibition at the Beirut Museum</v>
       </c>
-      <c r="F10" s="48"/>
-    </row>
-    <row r="11" spans="1:6" ht="27" x14ac:dyDescent="0.2">
+      <c r="F10" s="47"/>
+    </row>
+    <row r="11" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>2</v>
       </c>
@@ -3002,15 +2993,15 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E11" s="56" t="str" cm="1">
+      <c r="E11" s="55" t="str" cm="1">
         <f t="array" ref="E11">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1957/3/25–1957/7/21: Exhibition at the Beirut Museum
 1960/9/25–1960/10/1: Exhibition at the National Art Museum</v>
       </c>
-      <c r="F11" s="48"/>
-    </row>
-    <row r="12" spans="1:6" ht="183.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F11" s="47"/>
+    </row>
+    <row r="12" spans="1:6" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -3022,7 +3013,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>5</v>
       </c>
-      <c r="E12" s="56" t="str" cm="1">
+      <c r="E12" s="55" t="str" cm="1">
         <f t="array" ref="E12">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1951/1/1–2009/1/1: Exhibition at the Jordan Archaeological Museum
@@ -3031,9 +3022,9 @@
 1997/9/1–1997/9/18: Ancient Scrolls from the Dead Sea at the Brigham Young University Museum of Art
 2014/1/1–1900/1/0: Exhibition at the The Jordan Museum</v>
       </c>
-      <c r="F12" s="48"/>
-    </row>
-    <row r="13" spans="1:6" ht="351" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F12" s="47"/>
+    </row>
+    <row r="13" spans="1:6" ht="351" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -3045,7 +3036,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>10</v>
       </c>
-      <c r="E13" s="56" t="str" cm="1">
+      <c r="E13" s="55" t="str" cm="1">
         <f t="array" ref="E13">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1957/3/25–1957/7/21: Exhibition at the Beirut Museum
@@ -3059,9 +3050,9 @@
 1965/10/26–1965/11/15: Dead Sea Scrolls of Jordan at the Royal Ontario Museum
 1965/12/16–1966/1/29: Dead Sea Scrolls of Jordan at the British Museum</v>
       </c>
-      <c r="F13" s="48"/>
-    </row>
-    <row r="14" spans="1:6" ht="209" x14ac:dyDescent="0.2">
+      <c r="F13" s="47"/>
+    </row>
+    <row r="14" spans="1:6" ht="252" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -3075,7 +3066,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>9</v>
       </c>
-      <c r="E14" s="56" t="str" cm="1">
+      <c r="E14" s="55" t="str" cm="1">
         <f t="array" ref="E14">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1953/6/1–1953/11/1: From the Land of the Bible at the Metropolitan Museum of Art
@@ -3088,9 +3079,9 @@
 2003/6/17–2003/11/2: Archaeology and the Bible—From King David to the Dead Sea Scrolls at the Pointe-à-Callière
 2003/12/5–2004/4/12: Ancient Treasures and the Dead Sea Scrolls at the Canadian Museum of Civilization</v>
       </c>
-      <c r="F14" s="48"/>
-    </row>
-    <row r="15" spans="1:6" ht="27" x14ac:dyDescent="0.2">
+      <c r="F14" s="47"/>
+    </row>
+    <row r="15" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>2</v>
       </c>
@@ -3102,15 +3093,15 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E15" s="56" t="str" cm="1">
+      <c r="E15" s="55" t="str" cm="1">
         <f t="array" ref="E15">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1964/4/26–1964/5/10: The Book and the Spade at the Wisconsin Center
 1964/5/21–1964/6/7: The Book and the Spade at the Public Museum of Milwaukee</v>
       </c>
-      <c r="F15" s="48"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F15" s="47"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>2</v>
       </c>
@@ -3122,14 +3113,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E16" s="56" t="str" cm="1">
+      <c r="E16" s="55" t="str" cm="1">
         <f t="array" ref="E16">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1957/3/25–1957/7/21: Exhibition at the Beirut Museum</v>
       </c>
-      <c r="F16" s="48"/>
-    </row>
-    <row r="17" spans="1:6" ht="63" x14ac:dyDescent="0.2">
+      <c r="F16" s="47"/>
+    </row>
+    <row r="17" spans="1:6" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -3141,7 +3132,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>4</v>
       </c>
-      <c r="E17" s="56" t="str" cm="1">
+      <c r="E17" s="55" t="str" cm="1">
         <f t="array" ref="E17">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1964/4/26–1964/5/10: The Book and the Spade at the Wisconsin Center
@@ -3149,9 +3140,9 @@
 1971/6/19–1971/9/5: An Exhibition on the Dead Sea Scrolls at the American Bible Society
 1975/4/13–1975/5/4: The Book and the Spade at the Wisconsin Center</v>
       </c>
-      <c r="F17" s="48"/>
-    </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="F17" s="47"/>
+    </row>
+    <row r="18" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -3163,15 +3154,15 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E18" s="56" t="str" cm="1">
+      <c r="E18" s="55" t="str" cm="1">
         <f t="array" ref="E18">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1964/4/26–1964/5/10: The Book and the Spade at the Wisconsin Center
 1964/5/21–1964/6/7: The Book and the Spade at the Public Museum of Milwaukee</v>
       </c>
-      <c r="F18" s="48"/>
-    </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="F18" s="47"/>
+    </row>
+    <row r="19" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -3183,15 +3174,15 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E19" s="56" t="str" cm="1">
+      <c r="E19" s="55" t="str" cm="1">
         <f t="array" ref="E19">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1964/4/26–1964/5/10: The Book and the Spade at the Wisconsin Center
 1964/5/21–1964/6/7: The Book and the Spade at the Public Museum of Milwaukee</v>
       </c>
-      <c r="F19" s="48"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="47"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -3199,18 +3190,18 @@
         <v>258</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="43">
+      <c r="D20" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E20" s="56" t="str" cm="1">
+      <c r="E20" s="55" t="str" cm="1">
         <f t="array" ref="E20">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1951/1/1–2009/1/1: Exhibition at the Jordan Archaeological Museum</v>
       </c>
-      <c r="F20" s="48"/>
-    </row>
-    <row r="21" spans="1:6" ht="171" x14ac:dyDescent="0.2">
+      <c r="F20" s="47"/>
+    </row>
+    <row r="21" spans="1:6" ht="214.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -3222,7 +3213,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>13</v>
       </c>
-      <c r="E21" s="56" t="str" cm="1">
+      <c r="E21" s="55" t="str" cm="1">
         <f t="array" ref="E21">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1950/2/15–1950/2/15: Exhibition at the The British Museum
@@ -3239,89 +3230,89 @@
 2003/12/5–2004/4/12: Ancient Treasures and the Dead Sea Scrolls at the Canadian Museum of Civilization
 2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F21" s="48"/>
-    </row>
-    <row r="22" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F21" s="47"/>
+    </row>
+    <row r="22" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>251</v>
       </c>
       <c r="B22" s="22" t="s">
         <v>252</v>
       </c>
-      <c r="C22" s="46"/>
+      <c r="C22" s="45"/>
       <c r="D22" s="13">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E22" s="56" t="str" cm="1">
+      <c r="E22" s="55" t="str" cm="1">
         <f t="array" ref="E22">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2009/6/27–2010/1/3: Dead Sea Scrolls: Words that Changed the World at the Royal Ontario Museum</v>
       </c>
-      <c r="F22" s="48"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="45" t="s">
+      <c r="F22" s="47"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="43" t="s">
         <v>250</v>
       </c>
-      <c r="C23" s="46"/>
-      <c r="D23" s="51">
+      <c r="C23" s="45"/>
+      <c r="D23" s="50">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E23" s="56" t="str" cm="1">
+      <c r="E23" s="55" t="str" cm="1">
         <f t="array" ref="E23">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2009/6/27–2010/1/3: Dead Sea Scrolls: Words that Changed the World at the Royal Ontario Museum</v>
       </c>
-      <c r="F23" s="48"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="45" t="s">
+      <c r="F23" s="47"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="43" t="s">
         <v>249</v>
       </c>
-      <c r="C24" s="46"/>
+      <c r="C24" s="45"/>
       <c r="D24" s="13">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E24" s="56" t="str" cm="1">
+      <c r="E24" s="55" t="str" cm="1">
         <f t="array" ref="E24">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2009/6/27–2010/1/3: Dead Sea Scrolls: Words that Changed the World at the Royal Ontario Museum</v>
       </c>
-      <c r="F24" s="48"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F24" s="47"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="33" t="s">
         <v>248</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="52">
+      <c r="C25" s="35"/>
+      <c r="D25" s="51">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E25" s="56" t="str" cm="1">
+      <c r="E25" s="55" t="str" cm="1">
         <f t="array" ref="E25">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2009/6/27–2009/10/9: Dead Sea Scrolls: Words that Changed the World at the Royal Ontario Museum</v>
       </c>
-      <c r="F25" s="48"/>
-    </row>
-    <row r="26" spans="1:6" ht="171" x14ac:dyDescent="0.2">
-      <c r="A26" s="33" t="s">
+      <c r="F25" s="47"/>
+    </row>
+    <row r="26" spans="1:6" ht="156.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="33" t="s">
         <v>219</v>
       </c>
       <c r="C26" s="2"/>
@@ -3329,7 +3320,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>10</v>
       </c>
-      <c r="E26" s="56" t="str" cm="1">
+      <c r="E26" s="55" t="str" cm="1">
         <f t="array" ref="E26">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1953/6/1–1953/11/1: From the Land of the Bible at the Metropolitan Museum of Art
@@ -3343,9 +3334,9 @@
 1968/5/22–1968/7/3: From the Lands of the Bible at the America-Israel Culture House
 1975/4/13–1975/5/4: The Book and the Spade at the Wisconsin Center</v>
       </c>
-      <c r="F26" s="48"/>
-    </row>
-    <row r="27" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+      <c r="F26" s="47"/>
+    </row>
+    <row r="27" spans="1:6" ht="231" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -3353,11 +3344,11 @@
         <v>191</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="41">
+      <c r="D27" s="40">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>13</v>
       </c>
-      <c r="E27" s="56" t="str" cm="1">
+      <c r="E27" s="55" t="str" cm="1">
         <f t="array" ref="E27">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1949/10/22–1949/11/6: Ancient Hebrew Scrolls at the Library of Congress
@@ -3374,9 +3365,9 @@
 2014/11/4–2015/1/25: Temple, Scrolls, and Divine Messengers: Archaeology of the Land of Israel in Roman Times at the Chantal Miller Gallery
 2017/11/17–1900/1/0: Exhibition at the Museum of the Bible</v>
       </c>
-      <c r="F27" s="48"/>
-    </row>
-    <row r="28" spans="1:6" ht="268" x14ac:dyDescent="0.2">
+      <c r="F27" s="47"/>
+    </row>
+    <row r="28" spans="1:6" ht="272.25" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
@@ -3384,11 +3375,11 @@
         <v>5</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="42">
+      <c r="D28" s="41">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>16</v>
       </c>
-      <c r="E28" s="56" t="str" cm="1">
+      <c r="E28" s="55" t="str" cm="1">
         <f t="array" ref="E28">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1949/10/22–1949/11/6: Ancient Hebrew Scrolls at the Library of Congress
@@ -3408,9 +3399,9 @@
 2007/12/5–2008/6/4: The Dead Sea Scrolls and the Birth of Christianity at the War Memorial of Korea
 2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F28" s="48"/>
-    </row>
-    <row r="29" spans="1:6" ht="110" x14ac:dyDescent="0.2">
+      <c r="F28" s="47"/>
+    </row>
+    <row r="29" spans="1:6" ht="132" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
@@ -3424,7 +3415,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>6</v>
       </c>
-      <c r="E29" s="56" t="str" cm="1">
+      <c r="E29" s="55" t="str" cm="1">
         <f t="array" ref="E29">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1949/10/22–1949/11/6: Ancient Hebrew Scrolls at the Library of Congress
@@ -3434,9 +3425,9 @@
 1951/10/1–1951/10/3: Exhibition at the Worcester Museum of Art
 1951/11/1–1951/12/1: Exhibition at the Vassar College</v>
       </c>
-      <c r="F29" s="48"/>
-    </row>
-    <row r="30" spans="1:6" ht="227" x14ac:dyDescent="0.2">
+      <c r="F29" s="47"/>
+    </row>
+    <row r="30" spans="1:6" ht="288" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
@@ -3450,7 +3441,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>8</v>
       </c>
-      <c r="E30" s="56" t="str" cm="1">
+      <c r="E30" s="55" t="str" cm="1">
         <f t="array" ref="E30">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1993/4/29–1993/8/1: Scrolls from the Dead Sea: The Ancient Library of Qumran and Modern Scholarship at the Library of Congress
@@ -3462,9 +3453,9 @@
 2003/3/17–2003/3/23: The European Fine Art Fair at the MECC
 2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F30" s="48"/>
-    </row>
-    <row r="31" spans="1:6" ht="135" x14ac:dyDescent="0.2">
+      <c r="F30" s="47"/>
+    </row>
+    <row r="31" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>10</v>
       </c>
@@ -3476,7 +3467,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>8</v>
       </c>
-      <c r="E31" s="56" t="str" cm="1">
+      <c r="E31" s="55" t="str" cm="1">
         <f t="array" ref="E31">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2009/6/27–2009/10/9: Dead Sea Scrolls: Words that Changed the World at the Royal Ontario Museum
@@ -3488,9 +3479,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F31" s="48"/>
-    </row>
-    <row r="32" spans="1:6" ht="407" x14ac:dyDescent="0.2">
+      <c r="F31" s="47"/>
+    </row>
+    <row r="32" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>10</v>
       </c>
@@ -3504,7 +3495,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>20</v>
       </c>
-      <c r="E32" s="56" t="str" cm="1">
+      <c r="E32" s="55" t="str" cm="1">
         <f t="array" ref="E32">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1993/4/29–1993/8/1: Scrolls from the Dead Sea: The Ancient Library of Qumran and Modern Scholarship at the Library of Congress
@@ -3528,9 +3519,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F32" s="48"/>
-    </row>
-    <row r="33" spans="1:6" ht="220" x14ac:dyDescent="0.2">
+      <c r="F32" s="47"/>
+    </row>
+    <row r="33" spans="1:6" ht="206.25" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>174</v>
       </c>
@@ -3542,7 +3533,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>13</v>
       </c>
-      <c r="E33" s="56" t="str" cm="1">
+      <c r="E33" s="55" t="str" cm="1">
         <f t="array" ref="E33">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1951/1/1–2009/1/1: Exhibition at the Jordan Archaeological Museum
@@ -3559,9 +3550,9 @@
 1997/10/21–1998/1/10: Treasures from the Dead Sea at the Manchester Museum
 2014/1/1–1900/1/0: Exhibition at the The Jordan Museum</v>
       </c>
-      <c r="F33" s="48"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F33" s="47"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>156</v>
       </c>
@@ -3573,14 +3564,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E34" s="56" t="str" cm="1">
+      <c r="E34" s="55" t="str" cm="1">
         <f t="array" ref="E34">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2006/9/23–2007/1/7: Discovering the Dead Sea Scrolls at the Pacific Science Center</v>
       </c>
-      <c r="F34" s="48"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F34" s="47"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>156</v>
       </c>
@@ -3592,14 +3583,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E35" s="56" t="str" cm="1">
+      <c r="E35" s="55" t="str" cm="1">
         <f t="array" ref="E35">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2009/6/27–2010/1/3: Dead Sea Scrolls: Words that Changed the World at the Royal Ontario Museum</v>
       </c>
-      <c r="F35" s="48"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F35" s="47"/>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>156</v>
       </c>
@@ -3611,14 +3602,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E36" s="56" t="str" cm="1">
+      <c r="E36" s="55" t="str" cm="1">
         <f t="array" ref="E36">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2009/6/27–2009/10/9: Dead Sea Scrolls: Words that Changed the World at the Royal Ontario Museum</v>
       </c>
-      <c r="F36" s="48"/>
-    </row>
-    <row r="37" spans="1:6" ht="135" x14ac:dyDescent="0.2">
+      <c r="F36" s="47"/>
+    </row>
+    <row r="37" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>156</v>
       </c>
@@ -3630,7 +3621,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>8</v>
       </c>
-      <c r="E37" s="56" t="str" cm="1">
+      <c r="E37" s="55" t="str" cm="1">
         <f t="array" ref="E37">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2009/6/27–2009/10/9: Dead Sea Scrolls: Words that Changed the World at the Royal Ontario Museum
@@ -3642,9 +3633,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F37" s="48"/>
-    </row>
-    <row r="38" spans="1:6" ht="81" x14ac:dyDescent="0.2">
+      <c r="F37" s="47"/>
+    </row>
+    <row r="38" spans="1:6" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>156</v>
       </c>
@@ -3656,7 +3647,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>5</v>
       </c>
-      <c r="E38" s="56" t="str" cm="1">
+      <c r="E38" s="55" t="str" cm="1">
         <f t="array" ref="E38">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1951/1/1–2009/1/1: Exhibition at the Jordan Archaeological Museum
@@ -3665,9 +3656,9 @@
 2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary
 2014/1/1–1900/1/0: Exhibition at the The Jordan Museum</v>
       </c>
-      <c r="F38" s="48"/>
-    </row>
-    <row r="39" spans="1:6" ht="135" x14ac:dyDescent="0.2">
+      <c r="F38" s="47"/>
+    </row>
+    <row r="39" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>156</v>
       </c>
@@ -3679,7 +3670,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>8</v>
       </c>
-      <c r="E39" s="56" t="str" cm="1">
+      <c r="E39" s="55" t="str" cm="1">
         <f t="array" ref="E39">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2009/6/27–2009/10/9: Dead Sea Scrolls: Words that Changed the World at the Royal Ontario Museum
@@ -3691,9 +3682,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F39" s="48"/>
-    </row>
-    <row r="40" spans="1:6" ht="153" x14ac:dyDescent="0.2">
+      <c r="F39" s="47"/>
+    </row>
+    <row r="40" spans="1:6" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>156</v>
       </c>
@@ -3705,7 +3696,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>9</v>
       </c>
-      <c r="E40" s="56" t="str" cm="1">
+      <c r="E40" s="55" t="str" cm="1">
         <f t="array" ref="E40">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1965/2/27–1965/3/21: Dead Sea Scrolls of Jordan at the Smithsonian National Museum of Natural History
@@ -3718,9 +3709,9 @@
 1965/10/26–1965/11/15: Dead Sea Scrolls of Jordan at the Royal Ontario Museum
 1965/12/16–1966/1/29: Dead Sea Scrolls of Jordan at the British Museum</v>
       </c>
-      <c r="F40" s="48"/>
-    </row>
-    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="F40" s="47"/>
+    </row>
+    <row r="41" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>156</v>
       </c>
@@ -3732,16 +3723,16 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E41" s="56" t="str" cm="1">
+      <c r="E41" s="55" t="str" cm="1">
         <f t="array" ref="E41">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/7/14–2000/10/15: Exhibition at the Art Gallery of New South Wales
 2001/3/6–2001/6/17: Exhibition at the National Gallery of Victoria
 2003/2/16–2003/6/1: The Dead Sea Scrolls at the Public Museum of Grand Rapids</v>
       </c>
-      <c r="F41" s="48"/>
-    </row>
-    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="F41" s="47"/>
+    </row>
+    <row r="42" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>156</v>
       </c>
@@ -3753,16 +3744,16 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E42" s="56" t="str" cm="1">
+      <c r="E42" s="55" t="str" cm="1">
         <f t="array" ref="E42">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/7/14–2000/10/15: Exhibition at the Art Gallery of New South Wales
 2001/3/6–2001/6/17: Exhibition at the National Gallery of Victoria
 2003/2/16–2003/6/1: The Dead Sea Scrolls at the Public Museum of Grand Rapids</v>
       </c>
-      <c r="F42" s="48"/>
-    </row>
-    <row r="43" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="F42" s="47"/>
+    </row>
+    <row r="43" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>156</v>
       </c>
@@ -3774,16 +3765,16 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E43" s="56" t="str" cm="1">
+      <c r="E43" s="55" t="str" cm="1">
         <f t="array" ref="E43">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/7/14–2000/10/15: Exhibition at the Art Gallery of New South Wales
 2001/3/6–2001/6/17: Exhibition at the National Gallery of Victoria
 2003/2/16–2003/6/1: The Dead Sea Scrolls at the Public Museum of Grand Rapids</v>
       </c>
-      <c r="F43" s="48"/>
-    </row>
-    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="F43" s="47"/>
+    </row>
+    <row r="44" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>156</v>
       </c>
@@ -3795,16 +3786,16 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E44" s="56" t="str" cm="1">
+      <c r="E44" s="55" t="str" cm="1">
         <f t="array" ref="E44">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/7/14–2000/10/15: Exhibition at the Art Gallery of New South Wales
 2001/3/6–2001/6/17: Exhibition at the National Gallery of Victoria
 2003/2/16–2003/6/1: The Dead Sea Scrolls at the Public Museum of Grand Rapids</v>
       </c>
-      <c r="F44" s="48"/>
-    </row>
-    <row r="45" spans="1:6" ht="135" x14ac:dyDescent="0.2">
+      <c r="F44" s="47"/>
+    </row>
+    <row r="45" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>156</v>
       </c>
@@ -3816,7 +3807,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>8</v>
       </c>
-      <c r="E45" s="56" t="str" cm="1">
+      <c r="E45" s="55" t="str" cm="1">
         <f t="array" ref="E45">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2009/6/27–2010/1/3: Dead Sea Scrolls: Words that Changed the World at the Royal Ontario Museum
@@ -3828,9 +3819,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F45" s="48"/>
-    </row>
-    <row r="46" spans="1:6" ht="81" x14ac:dyDescent="0.2">
+      <c r="F45" s="47"/>
+    </row>
+    <row r="46" spans="1:6" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>156</v>
       </c>
@@ -3842,7 +3833,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>5</v>
       </c>
-      <c r="E46" s="56" t="str" cm="1">
+      <c r="E46" s="55" t="str" cm="1">
         <f t="array" ref="E46">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1951/1/1–2009/1/1: Exhibition at the Jordan Archaeological Museum
@@ -3851,9 +3842,9 @@
 2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary
 2014/1/1–1900/1/0: Exhibition at the The Jordan Museum</v>
       </c>
-      <c r="F46" s="48"/>
-    </row>
-    <row r="47" spans="1:6" ht="135" x14ac:dyDescent="0.2">
+      <c r="F46" s="47"/>
+    </row>
+    <row r="47" spans="1:6" ht="132" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>156</v>
       </c>
@@ -3865,7 +3856,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>8</v>
       </c>
-      <c r="E47" s="56" t="str" cm="1">
+      <c r="E47" s="55" t="str" cm="1">
         <f t="array" ref="E47">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1993/4/29–1993/8/1: Scrolls from the Dead Sea: The Ancient Library of Qumran and Modern Scholarship at the Library of Congress
@@ -3877,9 +3868,9 @@
 2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum
 2006/9/23–2007/1/7: Discovering the Dead Sea Scrolls at the Pacific Science Center</v>
       </c>
-      <c r="F47" s="48"/>
-    </row>
-    <row r="48" spans="1:6" ht="220" x14ac:dyDescent="0.2">
+      <c r="F47" s="47"/>
+    </row>
+    <row r="48" spans="1:6" ht="206.25" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>156</v>
       </c>
@@ -3891,7 +3882,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>13</v>
       </c>
-      <c r="E48" s="56" t="str" cm="1">
+      <c r="E48" s="55" t="str" cm="1">
         <f t="array" ref="E48">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1965/2/27–1965/3/21: Dead Sea Scrolls of Jordan at the Smithsonian National Museum of Natural History
@@ -3908,9 +3899,9 @@
 2001/3/6–2001/6/17: Exhibition at the National Gallery of Victoria
 2003/2/16–2003/6/1: The Dead Sea Scrolls at the Public Museum of Grand Rapids</v>
       </c>
-      <c r="F48" s="48"/>
-    </row>
-    <row r="49" spans="1:6" ht="153" x14ac:dyDescent="0.2">
+      <c r="F48" s="47"/>
+    </row>
+    <row r="49" spans="1:6" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>156</v>
       </c>
@@ -3922,7 +3913,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>9</v>
       </c>
-      <c r="E49" s="56" t="str" cm="1">
+      <c r="E49" s="55" t="str" cm="1">
         <f t="array" ref="E49">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1965/2/27–1965/3/21: Dead Sea Scrolls of Jordan at the Smithsonian National Museum of Natural History
@@ -3935,9 +3926,9 @@
 1965/10/26–1965/11/15: Dead Sea Scrolls of Jordan at the Royal Ontario Museum
 1965/12/16–1966/1/29: Dead Sea Scrolls of Jordan at the British Museum</v>
       </c>
-      <c r="F49" s="48"/>
-    </row>
-    <row r="50" spans="1:6" ht="99" x14ac:dyDescent="0.2">
+      <c r="F49" s="47"/>
+    </row>
+    <row r="50" spans="1:6" ht="99" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>156</v>
       </c>
@@ -3949,7 +3940,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>6</v>
       </c>
-      <c r="E50" s="56" t="str" cm="1">
+      <c r="E50" s="55" t="str" cm="1">
         <f t="array" ref="E50">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1951/1/1–2009/1/1: Exhibition at the Jordan Archaeological Museum
@@ -3959,9 +3950,9 @@
 2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary
 2014/1/1–1900/1/0: Exhibition at the The Jordan Museum</v>
       </c>
-      <c r="F50" s="48"/>
-    </row>
-    <row r="51" spans="1:6" ht="117" x14ac:dyDescent="0.2">
+      <c r="F50" s="47"/>
+    </row>
+    <row r="51" spans="1:6" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>156</v>
       </c>
@@ -3973,7 +3964,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>7</v>
       </c>
-      <c r="E51" s="56" t="str" cm="1">
+      <c r="E51" s="55" t="str" cm="1">
         <f t="array" ref="E51">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1993/4/29–1993/8/1: Scrolls from the Dead Sea: The Ancient Library of Qumran and Modern Scholarship at the Library of Congress
@@ -3984,9 +3975,9 @@
 1999/5/7–1999/8/8: Die Schriftrollen vom Toten Meer at the Stiftsbibliotek
 2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
-      <c r="F51" s="48"/>
-    </row>
-    <row r="52" spans="1:6" ht="117" x14ac:dyDescent="0.2">
+      <c r="F51" s="47"/>
+    </row>
+    <row r="52" spans="1:6" ht="107.25" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>156</v>
       </c>
@@ -3998,7 +3989,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>7</v>
       </c>
-      <c r="E52" s="56" t="str" cm="1">
+      <c r="E52" s="55" t="str" cm="1">
         <f t="array" ref="E52">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2011/10/28–2012/4/15: Dead Sea Scrolls: Life and Faith in Ancient Times at the Discovery Times Square
@@ -4009,9 +4000,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F52" s="48"/>
-    </row>
-    <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="F52" s="47"/>
+    </row>
+    <row r="53" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>156</v>
       </c>
@@ -4023,16 +4014,16 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E53" s="56" t="str" cm="1">
+      <c r="E53" s="55" t="str" cm="1">
         <f t="array" ref="E53">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/7/14–2000/10/15: Exhibition at the Art Gallery of New South Wales
 2001/3/6–2001/6/17: Exhibition at the National Gallery of Victoria
 2003/2/16–2003/6/1: The Dead Sea Scrolls at the Public Museum of Grand Rapids</v>
       </c>
-      <c r="F53" s="48"/>
-    </row>
-    <row r="54" spans="1:6" ht="268" x14ac:dyDescent="0.2">
+      <c r="F53" s="47"/>
+    </row>
+    <row r="54" spans="1:6" ht="255.75" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>156</v>
       </c>
@@ -4044,7 +4035,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>16</v>
       </c>
-      <c r="E54" s="56" t="str" cm="1">
+      <c r="E54" s="55" t="str" cm="1">
         <f t="array" ref="E54">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1965/2/27–1965/3/21: Dead Sea Scrolls of Jordan at the Smithsonian National Museum of Natural History
@@ -4064,9 +4055,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F54" s="48"/>
-    </row>
-    <row r="55" spans="1:6" ht="252" x14ac:dyDescent="0.2">
+      <c r="F54" s="47"/>
+    </row>
+    <row r="55" spans="1:6" ht="239.25" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>156</v>
       </c>
@@ -4080,7 +4071,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>15</v>
       </c>
-      <c r="E55" s="56" t="str" cm="1">
+      <c r="E55" s="55" t="str" cm="1">
         <f t="array" ref="E55">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1964/4/22–1964/10/18: Exhibition at the New York World's Fair
@@ -4099,9 +4090,9 @@
 2001/3/6–2001/6/17: Exhibition at the National Gallery of Victoria
 2003/2/16–2003/6/1: The Dead Sea Scrolls at the Public Museum of Grand Rapids</v>
       </c>
-      <c r="F55" s="48"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F55" s="47"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>156</v>
       </c>
@@ -4113,14 +4104,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E56" s="56" t="str" cm="1">
+      <c r="E56" s="55" t="str" cm="1">
         <f t="array" ref="E56">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
-      <c r="F56" s="48"/>
-    </row>
-    <row r="57" spans="1:6" ht="117" x14ac:dyDescent="0.2">
+      <c r="F56" s="47"/>
+    </row>
+    <row r="57" spans="1:6" ht="107.25" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>156</v>
       </c>
@@ -4132,7 +4123,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>7</v>
       </c>
-      <c r="E57" s="56" t="str" cm="1">
+      <c r="E57" s="55" t="str" cm="1">
         <f t="array" ref="E57">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2011/10/28–2012/4/15: Dead Sea Scrolls: Life and Faith in Ancient Times at the Discovery Times Square
@@ -4143,9 +4134,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F57" s="48"/>
-    </row>
-    <row r="58" spans="1:6" ht="236" x14ac:dyDescent="0.2">
+      <c r="F57" s="47"/>
+    </row>
+    <row r="58" spans="1:6" ht="231" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>156</v>
       </c>
@@ -4157,7 +4148,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>14</v>
       </c>
-      <c r="E58" s="56" t="str" cm="1">
+      <c r="E58" s="55" t="str" cm="1">
         <f t="array" ref="E58">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1993/4/29–1993/8/1: Scrolls from the Dead Sea: The Ancient Library of Qumran and Modern Scholarship at the Library of Congress
@@ -4175,9 +4166,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F58" s="48"/>
-    </row>
-    <row r="59" spans="1:6" ht="63" x14ac:dyDescent="0.2">
+      <c r="F58" s="47"/>
+    </row>
+    <row r="59" spans="1:6" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>156</v>
       </c>
@@ -4189,7 +4180,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>4</v>
       </c>
-      <c r="E59" s="56" t="str" cm="1">
+      <c r="E59" s="55" t="str" cm="1">
         <f t="array" ref="E59">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/7/14–2000/10/15: Exhibition at the Art Gallery of New South Wales
@@ -4197,9 +4188,9 @@
 2003/2/16–2003/6/1: The Dead Sea Scrolls at the Public Museum of Grand Rapids
 2006/9/23–2007/1/7: Discovering the Dead Sea Scrolls at the Pacific Science Center</v>
       </c>
-      <c r="F59" s="48"/>
-    </row>
-    <row r="60" spans="1:6" ht="188" x14ac:dyDescent="0.2">
+      <c r="F59" s="47"/>
+    </row>
+    <row r="60" spans="1:6" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>156</v>
       </c>
@@ -4211,7 +4202,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>11</v>
       </c>
-      <c r="E60" s="56" t="str" cm="1">
+      <c r="E60" s="55" t="str" cm="1">
         <f t="array" ref="E60">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/7/14–2000/10/15: Exhibition at the Art Gallery of New South Wales
@@ -4226,9 +4217,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F60" s="48"/>
-    </row>
-    <row r="61" spans="1:6" ht="117" x14ac:dyDescent="0.2">
+      <c r="F60" s="47"/>
+    </row>
+    <row r="61" spans="1:6" ht="107.25" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>156</v>
       </c>
@@ -4240,7 +4231,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>7</v>
       </c>
-      <c r="E61" s="56" t="str" cm="1">
+      <c r="E61" s="55" t="str" cm="1">
         <f t="array" ref="E61">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2011/10/28–2012/4/15: Dead Sea Scrolls: Life and Faith in Ancient Times at the Discovery Times Square
@@ -4251,9 +4242,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F61" s="48"/>
-    </row>
-    <row r="62" spans="1:6" ht="99" x14ac:dyDescent="0.2">
+      <c r="F61" s="47"/>
+    </row>
+    <row r="62" spans="1:6" ht="99" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>156</v>
       </c>
@@ -4265,7 +4256,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>6</v>
       </c>
-      <c r="E62" s="56" t="str" cm="1">
+      <c r="E62" s="55" t="str" cm="1">
         <f t="array" ref="E62">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1993/4/29–1993/8/1: Scrolls from the Dead Sea: The Ancient Library of Qumran and Modern Scholarship at the Library of Congress
@@ -4275,9 +4266,9 @@
 1998/11/14–1999/4/18: Qumran – Die Schriftrollen vom Toten Meer at the Roemisch Germanisches Museum
 2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
-      <c r="F62" s="48"/>
-    </row>
-    <row r="63" spans="1:6" ht="117" x14ac:dyDescent="0.2">
+      <c r="F62" s="47"/>
+    </row>
+    <row r="63" spans="1:6" ht="115.5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>156</v>
       </c>
@@ -4289,7 +4280,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>7</v>
       </c>
-      <c r="E63" s="56" t="str" cm="1">
+      <c r="E63" s="55" t="str" cm="1">
         <f t="array" ref="E63">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1993/4/29–1993/8/1: Scrolls from the Dead Sea: The Ancient Library of Qumran and Modern Scholarship at the Library of Congress
@@ -4300,9 +4291,9 @@
 2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum
 2006/9/23–2007/1/7: Discovering the Dead Sea Scrolls at the Pacific Science Center</v>
       </c>
-      <c r="F63" s="48"/>
-    </row>
-    <row r="64" spans="1:6" ht="117" x14ac:dyDescent="0.2">
+      <c r="F63" s="47"/>
+    </row>
+    <row r="64" spans="1:6" ht="107.25" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>156</v>
       </c>
@@ -4314,7 +4305,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>7</v>
       </c>
-      <c r="E64" s="56" t="str" cm="1">
+      <c r="E64" s="55" t="str" cm="1">
         <f t="array" ref="E64">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2011/10/28–2012/4/15: Dead Sea Scrolls: Life and Faith in Ancient Times at the Discovery Times Square
@@ -4325,9 +4316,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F64" s="48"/>
-    </row>
-    <row r="65" spans="1:6" ht="99" x14ac:dyDescent="0.2">
+      <c r="F64" s="47"/>
+    </row>
+    <row r="65" spans="1:6" ht="99" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>156</v>
       </c>
@@ -4339,7 +4330,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>6</v>
       </c>
-      <c r="E65" s="56" t="str" cm="1">
+      <c r="E65" s="55" t="str" cm="1">
         <f t="array" ref="E65">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1993/4/29–1993/8/1: Scrolls from the Dead Sea: The Ancient Library of Qumran and Modern Scholarship at the Library of Congress
@@ -4349,9 +4340,9 @@
 1999/5/7–1999/8/8: Die Schriftrollen vom Toten Meer at the Stiftsbibliotek
 2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
-      <c r="F65" s="48"/>
-    </row>
-    <row r="66" spans="1:6" ht="63" x14ac:dyDescent="0.2">
+      <c r="F65" s="47"/>
+    </row>
+    <row r="66" spans="1:6" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>156</v>
       </c>
@@ -4363,7 +4354,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>4</v>
       </c>
-      <c r="E66" s="56" t="str" cm="1">
+      <c r="E66" s="55" t="str" cm="1">
         <f t="array" ref="E66">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/7/14–2000/10/15: Exhibition at the Art Gallery of New South Wales
@@ -4371,9 +4362,9 @@
 2003/2/16–2003/6/1: The Dead Sea Scrolls at the Public Museum of Grand Rapids
 2006/9/23–2007/1/7: Discovering the Dead Sea Scrolls at the Pacific Science Center</v>
       </c>
-      <c r="F66" s="48"/>
-    </row>
-    <row r="67" spans="1:6" ht="188" x14ac:dyDescent="0.2">
+      <c r="F66" s="47"/>
+    </row>
+    <row r="67" spans="1:6" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>156</v>
       </c>
@@ -4385,7 +4376,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>11</v>
       </c>
-      <c r="E67" s="56" t="str" cm="1">
+      <c r="E67" s="55" t="str" cm="1">
         <f t="array" ref="E67">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/7/14–2000/10/15: Exhibition at the Art Gallery of New South Wales
@@ -4400,9 +4391,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F67" s="48"/>
-    </row>
-    <row r="68" spans="1:6" ht="27" x14ac:dyDescent="0.2">
+      <c r="F67" s="47"/>
+    </row>
+    <row r="68" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>156</v>
       </c>
@@ -4414,15 +4405,15 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E68" s="56" t="str" cm="1">
+      <c r="E68" s="55" t="str" cm="1">
         <f t="array" ref="E68">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/7/14–2000/10/15: Exhibition at the Art Gallery of New South Wales
 2001/3/6–2001/6/17: Exhibition at the National Gallery of Victoria</v>
       </c>
-      <c r="F68" s="48"/>
-    </row>
-    <row r="69" spans="1:6" ht="99" x14ac:dyDescent="0.2">
+      <c r="F68" s="47"/>
+    </row>
+    <row r="69" spans="1:6" ht="99" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>156</v>
       </c>
@@ -4434,7 +4425,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>6</v>
       </c>
-      <c r="E69" s="56" t="str" cm="1">
+      <c r="E69" s="55" t="str" cm="1">
         <f t="array" ref="E69">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1993/4/29–1993/8/1: Scrolls from the Dead Sea: The Ancient Library of Qumran and Modern Scholarship at the Library of Congress
@@ -4444,9 +4435,9 @@
 1999/5/7–1999/8/8: Die Schriftrollen vom Toten Meer at the Stiftsbibliotek
 2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
-      <c r="F69" s="48"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F69" s="47"/>
+    </row>
+    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>156</v>
       </c>
@@ -4458,14 +4449,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E70" s="56" t="str" cm="1">
+      <c r="E70" s="55" t="str" cm="1">
         <f t="array" ref="E70">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2006/9/23–2007/1/7: Discovering the Dead Sea Scrolls at the Pacific Science Center</v>
       </c>
-      <c r="F70" s="48"/>
-    </row>
-    <row r="71" spans="1:6" ht="27" x14ac:dyDescent="0.2">
+      <c r="F70" s="47"/>
+    </row>
+    <row r="71" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>156</v>
       </c>
@@ -4477,15 +4468,15 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E71" s="56" t="str" cm="1">
+      <c r="E71" s="55" t="str" cm="1">
         <f t="array" ref="E71">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1993/10/2–1994/1/4: The Dead Sea Scrolls at the New York Public Library
 1994/2/26–1994/5/29: The Mystery of the Dead Sea Scrolls at the Fine Arts Museum</v>
       </c>
-      <c r="F71" s="48"/>
-    </row>
-    <row r="72" spans="1:6" ht="27" x14ac:dyDescent="0.2">
+      <c r="F71" s="47"/>
+    </row>
+    <row r="72" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>156</v>
       </c>
@@ -4497,15 +4488,15 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E72" s="56" t="str" cm="1">
+      <c r="E72" s="55" t="str" cm="1">
         <f t="array" ref="E72">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1993/4/29–1993/8/1: Scrolls from the Dead Sea: The Ancient Library of Qumran and Modern Scholarship at the Library of Congress
 1999/5/7–1999/8/8: Die Schriftrollen vom Toten Meer at the Stiftsbibliotek</v>
       </c>
-      <c r="F72" s="48"/>
-    </row>
-    <row r="73" spans="1:6" ht="204" x14ac:dyDescent="0.2">
+      <c r="F72" s="47"/>
+    </row>
+    <row r="73" spans="1:6" ht="189.75" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>156</v>
       </c>
@@ -4517,7 +4508,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>12</v>
       </c>
-      <c r="E73" s="56" t="str" cm="1">
+      <c r="E73" s="55" t="str" cm="1">
         <f t="array" ref="E73">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1965/2/27–1965/3/21: Dead Sea Scrolls of Jordan at the Smithsonian National Museum of Natural History
@@ -4533,9 +4524,9 @@
 2009/6/27–2010/1/3: Dead Sea Scrolls: Words that Changed the World at the Royal Ontario Museum
 2012/11/16–2013/4/14: Dead Sea Scrolls: Life and Faith in Ancient Times at the Cincinnati Museum Center</v>
       </c>
-      <c r="F73" s="48"/>
-    </row>
-    <row r="74" spans="1:6" ht="117" x14ac:dyDescent="0.2">
+      <c r="F73" s="47"/>
+    </row>
+    <row r="74" spans="1:6" ht="107.25" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>156</v>
       </c>
@@ -4547,7 +4538,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>7</v>
       </c>
-      <c r="E74" s="56" t="str" cm="1">
+      <c r="E74" s="55" t="str" cm="1">
         <f t="array" ref="E74">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2011/10/28–2012/4/15: Dead Sea Scrolls: Life and Faith in Ancient Times at the Discovery Times Square
@@ -4558,9 +4549,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F74" s="48"/>
-    </row>
-    <row r="75" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="F74" s="47"/>
+    </row>
+    <row r="75" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>156</v>
       </c>
@@ -4572,16 +4563,16 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E75" s="56" t="str" cm="1">
+      <c r="E75" s="55" t="str" cm="1">
         <f t="array" ref="E75">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/7/14–2000/10/15: Exhibition at the Art Gallery of New South Wales
 2001/3/6–2001/6/17: Exhibition at the National Gallery of Victoria
 2003/2/16–2003/6/1: The Dead Sea Scrolls at the Public Museum of Grand Rapids</v>
       </c>
-      <c r="F75" s="48"/>
-    </row>
-    <row r="76" spans="1:6" ht="135" x14ac:dyDescent="0.2">
+      <c r="F75" s="47"/>
+    </row>
+    <row r="76" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>156</v>
       </c>
@@ -4593,7 +4584,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>8</v>
       </c>
-      <c r="E76" s="56" t="str" cm="1">
+      <c r="E76" s="55" t="str" cm="1">
         <f t="array" ref="E76">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2009/6/27–2010/1/3: Dead Sea Scrolls: Words that Changed the World at the Royal Ontario Museum
@@ -4605,9 +4596,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F76" s="48"/>
-    </row>
-    <row r="77" spans="1:6" ht="99" x14ac:dyDescent="0.2">
+      <c r="F76" s="47"/>
+    </row>
+    <row r="77" spans="1:6" ht="99" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>156</v>
       </c>
@@ -4619,7 +4610,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>6</v>
       </c>
-      <c r="E77" s="56" t="str" cm="1">
+      <c r="E77" s="55" t="str" cm="1">
         <f t="array" ref="E77">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1993/4/29–1993/8/1: Scrolls from the Dead Sea: The Ancient Library of Qumran and Modern Scholarship at the Library of Congress
@@ -4629,9 +4620,9 @@
 1999/5/7–1999/8/8: Die Schriftrollen vom Toten Meer at the Stiftsbibliotek
 2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
-      <c r="F77" s="48"/>
-    </row>
-    <row r="78" spans="1:6" ht="117" x14ac:dyDescent="0.2">
+      <c r="F77" s="47"/>
+    </row>
+    <row r="78" spans="1:6" ht="107.25" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>156</v>
       </c>
@@ -4643,7 +4634,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>7</v>
       </c>
-      <c r="E78" s="56" t="str" cm="1">
+      <c r="E78" s="55" t="str" cm="1">
         <f t="array" ref="E78">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2011/10/28–2012/4/15: Dead Sea Scrolls: Life and Faith in Ancient Times at the Discovery Times Square
@@ -4654,9 +4645,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F78" s="48"/>
-    </row>
-    <row r="79" spans="1:6" ht="268" x14ac:dyDescent="0.2">
+      <c r="F78" s="47"/>
+    </row>
+    <row r="79" spans="1:6" ht="255.75" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>156</v>
       </c>
@@ -4668,7 +4659,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>16</v>
       </c>
-      <c r="E79" s="56" t="str" cm="1">
+      <c r="E79" s="55" t="str" cm="1">
         <f t="array" ref="E79">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1965/2/27–1965/3/21: Dead Sea Scrolls of Jordan at the Smithsonian National Museum of Natural History
@@ -4688,9 +4679,9 @@
 2015/3/10–2015/9/7: Dead Sea Scrolls: Life and Faith in Ancient Times at the California Science Center
 2018/3/16–2018/9/3: Dead Sea Scrolls: Life and Faith in Ancient Times at the Denver Museum of Nature and Science</v>
       </c>
-      <c r="F79" s="48"/>
-    </row>
-    <row r="80" spans="1:6" ht="27" x14ac:dyDescent="0.2">
+      <c r="F79" s="47"/>
+    </row>
+    <row r="80" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>156</v>
       </c>
@@ -4702,15 +4693,15 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E80" s="56" t="str" cm="1">
+      <c r="E80" s="55" t="str" cm="1">
         <f t="array" ref="E80">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum
 2009/6/27–2009/10/9: Dead Sea Scrolls: Words that Changed the World at the Royal Ontario Museum</v>
       </c>
-      <c r="F80" s="48"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F80" s="47"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>156</v>
       </c>
@@ -4722,14 +4713,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E81" s="56" t="str" cm="1">
+      <c r="E81" s="55" t="str" cm="1">
         <f t="array" ref="E81">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
-      <c r="F81" s="48"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F81" s="47"/>
+    </row>
+    <row r="82" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>156</v>
       </c>
@@ -4741,14 +4732,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E82" s="56" t="str" cm="1">
+      <c r="E82" s="55" t="str" cm="1">
         <f t="array" ref="E82">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2006/9/23–2007/1/7: Discovering the Dead Sea Scrolls at the Pacific Science Center</v>
       </c>
-      <c r="F82" s="49"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F82" s="48"/>
+    </row>
+    <row r="83" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>156</v>
       </c>
@@ -4760,14 +4751,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E83" s="56" t="str" cm="1">
+      <c r="E83" s="55" t="str" cm="1">
         <f t="array" ref="E83">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2006/9/23–2007/1/7: Discovering the Dead Sea Scrolls at the Pacific Science Center</v>
       </c>
-      <c r="F83" s="49"/>
-    </row>
-    <row r="84" spans="1:6" ht="153" x14ac:dyDescent="0.2">
+      <c r="F83" s="48"/>
+    </row>
+    <row r="84" spans="1:6" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>156</v>
       </c>
@@ -4779,7 +4770,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>9</v>
       </c>
-      <c r="E84" s="56" t="str" cm="1">
+      <c r="E84" s="55" t="str" cm="1">
         <f t="array" ref="E84">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1965/2/27–1965/3/21: Dead Sea Scrolls of Jordan at the Smithsonian National Museum of Natural History
@@ -4792,9 +4783,9 @@
 1965/10/26–1965/11/15: Dead Sea Scrolls of Jordan at the Royal Ontario Museum
 1965/12/16–1966/1/29: Dead Sea Scrolls of Jordan at the British Museum</v>
       </c>
-      <c r="F84" s="48"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F84" s="47"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>170</v>
       </c>
@@ -4806,14 +4797,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E85" s="56" t="str" cm="1">
+      <c r="E85" s="55" t="str" cm="1">
         <f t="array" ref="E85">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
-      <c r="F85" s="48"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F85" s="47"/>
+    </row>
+    <row r="86" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>12</v>
       </c>
@@ -4825,14 +4816,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E86" s="56" t="str" cm="1">
+      <c r="E86" s="55" t="str" cm="1">
         <f t="array" ref="E86">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F86" s="48"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F86" s="47"/>
+    </row>
+    <row r="87" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>12</v>
       </c>
@@ -4844,14 +4835,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E87" s="56" t="str" cm="1">
+      <c r="E87" s="55" t="str" cm="1">
         <f t="array" ref="E87">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F87" s="48"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F87" s="47"/>
+    </row>
+    <row r="88" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>12</v>
       </c>
@@ -4863,14 +4854,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E88" s="56" t="str" cm="1">
+      <c r="E88" s="55" t="str" cm="1">
         <f t="array" ref="E88">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F88" s="48"/>
-    </row>
-    <row r="89" spans="1:6" ht="63" x14ac:dyDescent="0.2">
+      <c r="F88" s="47"/>
+    </row>
+    <row r="89" spans="1:6" ht="66" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>12</v>
       </c>
@@ -4882,7 +4873,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>4</v>
       </c>
-      <c r="E89" s="56" t="str" cm="1">
+      <c r="E89" s="55" t="str" cm="1">
         <f t="array" ref="E89">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1997/9/1–1997/9/18: Ancient Scrolls from the Dead Sea at the Brigham Young University Museum of Art
@@ -4890,9 +4881,9 @@
 2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary
 2017/11/17–1900/1/0: Exhibition at the Museum of the Bible</v>
       </c>
-      <c r="F89" s="48"/>
-    </row>
-    <row r="90" spans="1:6" ht="63" x14ac:dyDescent="0.2">
+      <c r="F89" s="47"/>
+    </row>
+    <row r="90" spans="1:6" ht="90.75" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>12</v>
       </c>
@@ -4900,11 +4891,11 @@
         <v>207</v>
       </c>
       <c r="C90" s="3"/>
-      <c r="D90" s="29">
+      <c r="D90" s="28">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>5</v>
       </c>
-      <c r="E90" s="56" t="str" cm="1">
+      <c r="E90" s="55" t="str" cm="1">
         <f t="array" ref="E90">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1997/9/1–1997/9/18: Ancient Scrolls from the Dead Sea at the Brigham Young University Museum of Art
@@ -4913,9 +4904,9 @@
 2014/11/4–2015/1/25: Temple, Scrolls, and Divine Messengers: Archaeology of the Land of Israel in Roman Times at the Chantal Miller Gallery
 2017/11/17–1900/1/0: Exhibition at the Museum of the Bible</v>
       </c>
-      <c r="F90" s="48"/>
-    </row>
-    <row r="91" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="F90" s="47"/>
+    </row>
+    <row r="91" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>12</v>
       </c>
@@ -4927,16 +4918,16 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E91" s="56" t="str" cm="1">
+      <c r="E91" s="55" t="str" cm="1">
         <f t="array" ref="E91">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1997/9/1–1997/9/18: Ancient Scrolls from the Dead Sea at the Brigham Young University Museum of Art
 2007/12/5–2008/6/4: The Dead Sea Scrolls and the Birth of Christianity at the War Memorial of Korea
 2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F91" s="48"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F91" s="47"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>12</v>
       </c>
@@ -4948,14 +4939,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E92" s="56" t="str" cm="1">
+      <c r="E92" s="55" t="str" cm="1">
         <f t="array" ref="E92">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2017/11/17–1900/1/0: Exhibition at the Museum of the Bible</v>
       </c>
-      <c r="F92" s="48"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F92" s="47"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>12</v>
       </c>
@@ -4963,18 +4954,18 @@
         <v>245</v>
       </c>
       <c r="C93" s="3"/>
-      <c r="D93" s="29">
+      <c r="D93" s="28">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E93" s="56" t="str" cm="1">
+      <c r="E93" s="55" t="str" cm="1">
         <f t="array" ref="E93">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2017/11/17–1900/1/0: Exhibition at the Museum of the Bible</v>
       </c>
-      <c r="F93" s="48"/>
-    </row>
-    <row r="94" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="F93" s="47"/>
+    </row>
+    <row r="94" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>12</v>
       </c>
@@ -4988,16 +4979,16 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E94" s="56" t="str" cm="1">
+      <c r="E94" s="55" t="str" cm="1">
         <f t="array" ref="E94">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2017/9/21–2017/9/22: Biblical Heritage Archive Traveling Museum at the Fairhaven Baptist College
 2017/10/28–2017/10/28: Biblical Heritage Archive Traveling Museum at the Waukesha County Expo Center
 2019/10/8–2019/10/9: Biblical Heritage Archive Traveling Museum at the VCY Headquarters</v>
       </c>
-      <c r="F94" s="48"/>
-    </row>
-    <row r="95" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="F94" s="47"/>
+    </row>
+    <row r="95" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>12</v>
       </c>
@@ -5011,16 +5002,16 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E95" s="56" t="str" cm="1">
+      <c r="E95" s="55" t="str" cm="1">
         <f t="array" ref="E95">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2017/9/21–2017/9/22: Biblical Heritage Archive Traveling Museum at the Fairhaven Baptist College
 2017/10/28–2017/10/28: Biblical Heritage Archive Traveling Museum at the Waukesha County Expo Center
 2019/10/8–2019/10/9: Biblical Heritage Archive Traveling Museum at the VCY Headquarters</v>
       </c>
-      <c r="F95" s="48"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F95" s="47"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>180</v>
       </c>
@@ -5032,14 +5023,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E96" s="56" t="str" cm="1">
+      <c r="E96" s="55" t="str" cm="1">
         <f t="array" ref="E96">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1997/9/1–1997/9/18: Ancient Scrolls from the Dead Sea at the Brigham Young University Museum of Art</v>
       </c>
-      <c r="F96" s="48"/>
-    </row>
-    <row r="97" spans="1:6" ht="81" x14ac:dyDescent="0.2">
+      <c r="F96" s="47"/>
+    </row>
+    <row r="97" spans="1:6" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>180</v>
       </c>
@@ -5051,7 +5042,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>5</v>
       </c>
-      <c r="E97" s="56" t="str" cm="1">
+      <c r="E97" s="55" t="str" cm="1">
         <f t="array" ref="E97">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1986/9/25–1987/1/4: Treasures from the Holy Land: Ancient Art from the Israel Museum at the Metropolitan Museum of Art
@@ -5060,9 +5051,9 @@
 1990/5/1–1990/9/1: Planets, Potions, Parchments at the David M. Stewart Museum
 1997/9/1–1997/9/18: Ancient Scrolls from the Dead Sea at the Brigham Young University Museum of Art</v>
       </c>
-      <c r="F97" s="48"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F97" s="47"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>180</v>
       </c>
@@ -5074,14 +5065,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E98" s="56" t="str" cm="1">
+      <c r="E98" s="55" t="str" cm="1">
         <f t="array" ref="E98">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1997/9/1–1997/9/18: Ancient Scrolls from the Dead Sea at the Brigham Young University Museum of Art</v>
       </c>
-      <c r="F98" s="48"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F98" s="47"/>
+    </row>
+    <row r="99" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>180</v>
       </c>
@@ -5093,14 +5084,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E99" s="56" t="str" cm="1">
+      <c r="E99" s="55" t="str" cm="1">
         <f t="array" ref="E99">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1997/9/1–1997/9/18: Ancient Scrolls from the Dead Sea at the Brigham Young University Museum of Art</v>
       </c>
-      <c r="F99" s="48"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F99" s="47"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>19</v>
       </c>
@@ -5114,14 +5105,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E100" s="56" t="str" cm="1">
+      <c r="E100" s="55" t="str" cm="1">
         <f t="array" ref="E100">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F100" s="48"/>
-    </row>
-    <row r="101" spans="1:6" ht="135" x14ac:dyDescent="0.2">
+      <c r="F100" s="47"/>
+    </row>
+    <row r="101" spans="1:6" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>19</v>
       </c>
@@ -5135,7 +5126,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>10</v>
       </c>
-      <c r="E101" s="56" t="str" cm="1">
+      <c r="E101" s="55" t="str" cm="1">
         <f t="array" ref="E101">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2005/2/5–2005/5/1: Ink &amp; Blood: Dead Sea Scrolls to the English Bible at the Knoxville Convention Center
@@ -5149,9 +5140,9 @@
 2022/11/7–2022/11/10: Exhibition at the Aguttes Auction House
 2022/11/14–2022/11/15: Exhibition at the Aguttes Auction House</v>
       </c>
-      <c r="F101" s="48"/>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F101" s="47"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>19</v>
       </c>
@@ -5163,14 +5154,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E102" s="56" t="str" cm="1">
+      <c r="E102" s="55" t="str" cm="1">
         <f t="array" ref="E102">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F102" s="48"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F102" s="47"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>19</v>
       </c>
@@ -5182,14 +5173,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E103" s="56" t="str" cm="1">
+      <c r="E103" s="55" t="str" cm="1">
         <f t="array" ref="E103">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F103" s="48"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F103" s="47"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>19</v>
       </c>
@@ -5203,14 +5194,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E104" s="56" t="str" cm="1">
+      <c r="E104" s="55" t="str" cm="1">
         <f t="array" ref="E104">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F104" s="48"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F104" s="47"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>19</v>
       </c>
@@ -5224,14 +5215,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E105" s="56" t="str" cm="1">
+      <c r="E105" s="55" t="str" cm="1">
         <f t="array" ref="E105">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F105" s="48"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F105" s="47"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>19</v>
       </c>
@@ -5243,14 +5234,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E106" s="56" t="str" cm="1">
+      <c r="E106" s="55" t="str" cm="1">
         <f t="array" ref="E106">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F106" s="48"/>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F106" s="47"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>19</v>
       </c>
@@ -5264,14 +5255,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E107" s="56" t="str" cm="1">
+      <c r="E107" s="55" t="str" cm="1">
         <f t="array" ref="E107">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F107" s="48"/>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F107" s="47"/>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>19</v>
       </c>
@@ -5285,14 +5276,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E108" s="56" t="str" cm="1">
+      <c r="E108" s="55" t="str" cm="1">
         <f t="array" ref="E108">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F108" s="48"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F108" s="47"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>19</v>
       </c>
@@ -5306,14 +5297,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E109" s="56" t="str" cm="1">
+      <c r="E109" s="55" t="str" cm="1">
         <f t="array" ref="E109">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F109" s="48"/>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F109" s="47"/>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>19</v>
       </c>
@@ -5327,14 +5318,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E110" s="56" t="str" cm="1">
+      <c r="E110" s="55" t="str" cm="1">
         <f t="array" ref="E110">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F110" s="48"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F110" s="47"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>19</v>
       </c>
@@ -5348,14 +5339,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E111" s="56" t="str" cm="1">
+      <c r="E111" s="55" t="str" cm="1">
         <f t="array" ref="E111">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F111" s="48"/>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F111" s="47"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>19</v>
       </c>
@@ -5369,14 +5360,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E112" s="56" t="str" cm="1">
+      <c r="E112" s="55" t="str" cm="1">
         <f t="array" ref="E112">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F112" s="48"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F112" s="47"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>19</v>
       </c>
@@ -5390,14 +5381,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E113" s="56" t="str" cm="1">
+      <c r="E113" s="55" t="str" cm="1">
         <f t="array" ref="E113">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F113" s="48"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F113" s="47"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>19</v>
       </c>
@@ -5411,14 +5402,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E114" s="56" t="str" cm="1">
+      <c r="E114" s="55" t="str" cm="1">
         <f t="array" ref="E114">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F114" s="48"/>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F114" s="47"/>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>19</v>
       </c>
@@ -5432,14 +5423,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E115" s="56" t="str" cm="1">
+      <c r="E115" s="55" t="str" cm="1">
         <f t="array" ref="E115">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F115" s="48"/>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F115" s="47"/>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>19</v>
       </c>
@@ -5453,14 +5444,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E116" s="56" t="str" cm="1">
+      <c r="E116" s="55" t="str" cm="1">
         <f t="array" ref="E116">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F116" s="48"/>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F116" s="47"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>19</v>
       </c>
@@ -5474,14 +5465,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E117" s="56" t="str" cm="1">
+      <c r="E117" s="55" t="str" cm="1">
         <f t="array" ref="E117">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F117" s="48"/>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F117" s="47"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>19</v>
       </c>
@@ -5493,14 +5484,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E118" s="56" t="str" cm="1">
+      <c r="E118" s="55" t="str" cm="1">
         <f t="array" ref="E118">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2009/2/1–2009/2/1: Dead Sea Scrolls to the Bible in America at the Christ Church of the Valley</v>
       </c>
-      <c r="F118" s="48"/>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F118" s="47"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>19</v>
       </c>
@@ -5514,14 +5505,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E119" s="56" t="str" cm="1">
+      <c r="E119" s="55" t="str" cm="1">
         <f t="array" ref="E119">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F119" s="48"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F119" s="47"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>19</v>
       </c>
@@ -5535,14 +5526,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E120" s="56" t="str" cm="1">
+      <c r="E120" s="55" t="str" cm="1">
         <f t="array" ref="E120">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F120" s="48"/>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F120" s="47"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>19</v>
       </c>
@@ -5556,14 +5547,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E121" s="56" t="str" cm="1">
+      <c r="E121" s="55" t="str" cm="1">
         <f t="array" ref="E121">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F121" s="48"/>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F121" s="47"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>19</v>
       </c>
@@ -5577,14 +5568,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E122" s="56" t="str" cm="1">
+      <c r="E122" s="55" t="str" cm="1">
         <f t="array" ref="E122">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F122" s="48"/>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F122" s="47"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>19</v>
       </c>
@@ -5598,14 +5589,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E123" s="56" t="str" cm="1">
+      <c r="E123" s="55" t="str" cm="1">
         <f t="array" ref="E123">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F123" s="48"/>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F123" s="47"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>19</v>
       </c>
@@ -5619,14 +5610,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E124" s="56" t="str" cm="1">
+      <c r="E124" s="55" t="str" cm="1">
         <f t="array" ref="E124">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F124" s="48"/>
-    </row>
-    <row r="125" spans="1:6" ht="27" x14ac:dyDescent="0.2">
+      <c r="F124" s="47"/>
+    </row>
+    <row r="125" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>19</v>
       </c>
@@ -5638,15 +5629,15 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E125" s="56" t="str" cm="1">
+      <c r="E125" s="55" t="str" cm="1">
         <f t="array" ref="E125">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2010/4/8–2010/5/15: Dead Sea Scrolls to the Bible in America at the Bayside Church Granite Bay Campus
 2010/5/21–2010/8/29: Treasures of the Bible: The Dead Sea Scrolls and Beyond at the Azusa Pacific University</v>
       </c>
-      <c r="F125" s="48"/>
-    </row>
-    <row r="126" spans="1:6" ht="27" x14ac:dyDescent="0.2">
+      <c r="F125" s="47"/>
+    </row>
+    <row r="126" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>19</v>
       </c>
@@ -5660,15 +5651,15 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E126" s="56" t="str" cm="1">
+      <c r="E126" s="55" t="str" cm="1">
         <f t="array" ref="E126">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2010/4/8–2010/5/15: Dead Sea Scrolls to the Bible in America at the Bayside Church Granite Bay Campus
 2010/5/21–2010/8/29: Treasures of the Bible: The Dead Sea Scrolls and Beyond at the Azusa Pacific University</v>
       </c>
-      <c r="F126" s="48"/>
-    </row>
-    <row r="127" spans="1:6" ht="27" x14ac:dyDescent="0.2">
+      <c r="F126" s="47"/>
+    </row>
+    <row r="127" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>19</v>
       </c>
@@ -5682,15 +5673,15 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E127" s="56" t="str" cm="1">
+      <c r="E127" s="55" t="str" cm="1">
         <f t="array" ref="E127">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2010/4/8–2010/5/15: Dead Sea Scrolls to the Bible in America at the Bayside Church Granite Bay Campus
 2010/5/21–2010/8/29: Treasures of the Bible: The Dead Sea Scrolls and Beyond at the Azusa Pacific University</v>
       </c>
-      <c r="F127" s="48"/>
-    </row>
-    <row r="128" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="F127" s="47"/>
+    </row>
+    <row r="128" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>19</v>
       </c>
@@ -5702,16 +5693,16 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E128" s="56" t="str" cm="1">
+      <c r="E128" s="55" t="str" cm="1">
         <f t="array" ref="E128">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2009/2/1–2009/2/1: Dead Sea Scrolls to the Bible in America at the Christ Church of the Valley
 2010/4/8–2010/5/15: Dead Sea Scrolls to the Bible in America at the Bayside Church Granite Bay Campus
 2010/5/21–2010/8/29: Treasures of the Bible: The Dead Sea Scrolls and Beyond at the Azusa Pacific University</v>
       </c>
-      <c r="F128" s="48"/>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F128" s="47"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>19</v>
       </c>
@@ -5725,14 +5716,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E129" s="56" t="str" cm="1">
+      <c r="E129" s="55" t="str" cm="1">
         <f t="array" ref="E129">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F129" s="48"/>
-    </row>
-    <row r="130" spans="1:6" ht="81" x14ac:dyDescent="0.2">
+      <c r="F129" s="47"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>19</v>
       </c>
@@ -5746,14 +5737,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E130" s="56" t="str" cm="1">
+      <c r="E130" s="55" t="str" cm="1">
         <f t="array" ref="E130">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F130" s="48"/>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F130" s="47"/>
+    </row>
+    <row r="131" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>19</v>
       </c>
@@ -5767,14 +5758,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E131" s="56" t="str" cm="1">
+      <c r="E131" s="55" t="str" cm="1">
         <f t="array" ref="E131">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F131" s="48"/>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F131" s="47"/>
+    </row>
+    <row r="132" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>19</v>
       </c>
@@ -5788,14 +5779,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E132" s="56" t="str" cm="1">
+      <c r="E132" s="55" t="str" cm="1">
         <f t="array" ref="E132">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F132" s="48"/>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F132" s="47"/>
+    </row>
+    <row r="133" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>19</v>
       </c>
@@ -5809,14 +5800,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E133" s="56" t="str" cm="1">
+      <c r="E133" s="55" t="str" cm="1">
         <f t="array" ref="E133">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F133" s="48"/>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F133" s="47"/>
+    </row>
+    <row r="134" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>19</v>
       </c>
@@ -5830,14 +5821,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E134" s="56" t="str" cm="1">
+      <c r="E134" s="55" t="str" cm="1">
         <f t="array" ref="E134">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F134" s="48"/>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F134" s="47"/>
+    </row>
+    <row r="135" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>19</v>
       </c>
@@ -5851,14 +5842,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E135" s="56" t="str" cm="1">
+      <c r="E135" s="55" t="str" cm="1">
         <f t="array" ref="E135">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F135" s="48"/>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F135" s="47"/>
+    </row>
+    <row r="136" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>19</v>
       </c>
@@ -5872,14 +5863,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E136" s="56" t="str" cm="1">
+      <c r="E136" s="55" t="str" cm="1">
         <f t="array" ref="E136">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F136" s="48"/>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F136" s="47"/>
+    </row>
+    <row r="137" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>19</v>
       </c>
@@ -5893,14 +5884,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E137" s="56" t="str" cm="1">
+      <c r="E137" s="55" t="str" cm="1">
         <f t="array" ref="E137">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F137" s="48"/>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F137" s="47"/>
+    </row>
+    <row r="138" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>19</v>
       </c>
@@ -5912,14 +5903,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E138" s="56" t="str" cm="1">
+      <c r="E138" s="55" t="str" cm="1">
         <f t="array" ref="E138">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F138" s="48"/>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F138" s="47"/>
+    </row>
+    <row r="139" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>19</v>
       </c>
@@ -5933,14 +5924,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E139" s="56" t="str" cm="1">
+      <c r="E139" s="55" t="str" cm="1">
         <f t="array" ref="E139">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F139" s="48"/>
-    </row>
-    <row r="140" spans="1:6" ht="27" x14ac:dyDescent="0.2">
+      <c r="F139" s="47"/>
+    </row>
+    <row r="140" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>19</v>
       </c>
@@ -5954,15 +5945,15 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E140" s="56" t="str" cm="1">
+      <c r="E140" s="55" t="str" cm="1">
         <f t="array" ref="E140">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary
 2013/1/14–1900/1/0: Exhibition at the Lanier Theological Library</v>
       </c>
-      <c r="F140" s="48"/>
-    </row>
-    <row r="141" spans="1:6" ht="135" x14ac:dyDescent="0.2">
+      <c r="F140" s="47"/>
+    </row>
+    <row r="141" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>19</v>
       </c>
@@ -5974,7 +5965,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>8</v>
       </c>
-      <c r="E141" s="56" t="str" cm="1">
+      <c r="E141" s="55" t="str" cm="1">
         <f t="array" ref="E141">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2011/4/7–2011/4/9: 400th Anniversary: The King James Bible and the World it Made at the Baylor University
@@ -5986,9 +5977,9 @@
 2015/3/3–2016/4/2: Passages at the 26565 Bouquet canyon rd
 2017/11/17–1900/1/0: Exhibition at the Museum of the Bible</v>
       </c>
-      <c r="F141" s="48"/>
-    </row>
-    <row r="142" spans="1:6" ht="63" x14ac:dyDescent="0.2">
+      <c r="F141" s="47"/>
+    </row>
+    <row r="142" spans="1:6" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>19</v>
       </c>
@@ -6002,7 +5993,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>4</v>
       </c>
-      <c r="E142" s="56" t="str" cm="1">
+      <c r="E142" s="55" t="str" cm="1">
         <f t="array" ref="E142">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2005/1/14–2005/3/27: Dead Sea Scrolls to the Bible in America at the Providence Place
@@ -6010,9 +6001,9 @@
 2009/8/28–2009/9/20: The Dead Sea Scrolls &amp; the Ancient World at the The Arts House
 2017/11/17–1900/1/0: Exhibition at the Museum of the Bible</v>
       </c>
-      <c r="F142" s="48"/>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F142" s="47"/>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>19</v>
       </c>
@@ -6026,14 +6017,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E143" s="56" t="str" cm="1">
+      <c r="E143" s="55" t="str" cm="1">
         <f t="array" ref="E143">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2009/8/28–2009/9/20: The Dead Sea Scrolls &amp; the Ancient World at the The Arts House</v>
       </c>
-      <c r="F143" s="48"/>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F143" s="47"/>
+    </row>
+    <row r="144" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>19</v>
       </c>
@@ -6047,14 +6038,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E144" s="56" t="str" cm="1">
+      <c r="E144" s="55" t="str" cm="1">
         <f t="array" ref="E144">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F144" s="48"/>
-    </row>
-    <row r="145" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="F144" s="47"/>
+    </row>
+    <row r="145" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>19</v>
       </c>
@@ -6068,16 +6059,16 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E145" s="56" t="str" cm="1">
+      <c r="E145" s="55" t="str" cm="1">
         <f t="array" ref="E145">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary
 2014/4/2–2014/6/22: Verbum Domini II at the Braccio di Carlo Magno museum
 2017/4/7–2017/5/13: Unser Buch at the Augsburger Rathaus</v>
       </c>
-      <c r="F145" s="48"/>
-    </row>
-    <row r="146" spans="1:6" ht="27" x14ac:dyDescent="0.2">
+      <c r="F145" s="47"/>
+    </row>
+    <row r="146" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>19</v>
       </c>
@@ -6091,57 +6082,57 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E146" s="56" t="str" cm="1">
+      <c r="E146" s="55" t="str" cm="1">
         <f t="array" ref="E146">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary
 2014/4/2–2014/6/22: Verbum Domini II at the Braccio di Carlo Magno museum</v>
       </c>
-      <c r="F146" s="48"/>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F146" s="47"/>
+    </row>
+    <row r="147" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B147" s="38" t="s">
+      <c r="B147" s="37" t="s">
         <v>134</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D147" s="43">
+      <c r="D147" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E147" s="56" t="str" cm="1">
+      <c r="E147" s="55" t="str" cm="1">
         <f t="array" ref="E147">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F147" s="48"/>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F147" s="47"/>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B148" s="38" t="s">
+      <c r="B148" s="37" t="s">
         <v>136</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D148" s="43" t="str">
+      <c r="D148" s="42" t="str">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E148" s="56" t="str" cm="1">
+      <c r="E148" s="55" t="str" cm="1">
         <f t="array" ref="E148">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F148" s="48"/>
-    </row>
-    <row r="149" spans="1:6" ht="305.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F148" s="47"/>
+    </row>
+    <row r="149" spans="1:6" ht="305.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
         <v>19</v>
       </c>
@@ -6155,7 +6146,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>4</v>
       </c>
-      <c r="E149" s="56" t="str" cm="1">
+      <c r="E149" s="55" t="str" cm="1">
         <f t="array" ref="E149">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2005/1/14–2005/3/27: Dead Sea Scrolls to the Bible in America at the Providence Place
@@ -6163,9 +6154,9 @@
 2009/8/28–2009/9/20: The Dead Sea Scrolls &amp; the Ancient World at the The Arts House
 2011/1/27–2011/5/1: Bible in English at the Gerber Academic Building at Ashland Theological Seminary</v>
       </c>
-      <c r="F149" s="48"/>
-    </row>
-    <row r="150" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="F149" s="47"/>
+    </row>
+    <row r="150" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
         <v>19</v>
       </c>
@@ -6179,16 +6170,16 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E150" s="56" t="str" cm="1">
+      <c r="E150" s="55" t="str" cm="1">
         <f t="array" ref="E150">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary
 2014/4/2–2014/6/22: Verbum Domini II at the Braccio di Carlo Magno museum
 2017/4/7–2017/5/13: Unser Buch at the Augsburger Rathaus</v>
       </c>
-      <c r="F150" s="48"/>
-    </row>
-    <row r="151" spans="1:6" ht="27" x14ac:dyDescent="0.2">
+      <c r="F150" s="47"/>
+    </row>
+    <row r="151" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
         <v>19</v>
       </c>
@@ -6202,15 +6193,15 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E151" s="56" t="str" cm="1">
+      <c r="E151" s="55" t="str" cm="1">
         <f t="array" ref="E151">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary
 2017/11/17–1900/1/0: Exhibition at the Museum of the Bible</v>
       </c>
-      <c r="F151" s="48"/>
-    </row>
-    <row r="152" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="F151" s="47"/>
+    </row>
+    <row r="152" spans="1:6" ht="41.25" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>19</v>
       </c>
@@ -6224,16 +6215,16 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E152" s="56" t="str" cm="1">
+      <c r="E152" s="55" t="str" cm="1">
         <f t="array" ref="E152">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2005/1/14–2005/3/27: Dead Sea Scrolls to the Bible in America at the Providence Place
 2005/4/27–2005/6/1: Dead Sea Scrolls to the Bible in America at the 
 2009/8/28–2009/9/20: The Dead Sea Scrolls &amp; the Ancient World at the The Arts House</v>
       </c>
-      <c r="F152" s="48"/>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F152" s="47"/>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
         <v>19</v>
       </c>
@@ -6247,14 +6238,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E153" s="56" t="str" cm="1">
+      <c r="E153" s="55" t="str" cm="1">
         <f t="array" ref="E153">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F153" s="48"/>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F153" s="47"/>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>19</v>
       </c>
@@ -6268,14 +6259,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E154" s="56" t="str" cm="1">
+      <c r="E154" s="55" t="str" cm="1">
         <f t="array" ref="E154">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F154" s="48"/>
-    </row>
-    <row r="155" spans="1:6" ht="28" x14ac:dyDescent="0.2">
+      <c r="F154" s="47"/>
+    </row>
+    <row r="155" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>19</v>
       </c>
@@ -6287,14 +6278,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E155" s="56" t="str" cm="1">
+      <c r="E155" s="55" t="str" cm="1">
         <f t="array" ref="E155">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F155" s="48"/>
-    </row>
-    <row r="156" spans="1:6" ht="135" x14ac:dyDescent="0.2">
+      <c r="F155" s="47"/>
+    </row>
+    <row r="156" spans="1:6" ht="123.75" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>19</v>
       </c>
@@ -6308,7 +6299,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>8</v>
       </c>
-      <c r="E156" s="56" t="str" cm="1">
+      <c r="E156" s="55" t="str" cm="1">
         <f t="array" ref="E156">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2003/4/6–2003/4/29: From the Dead Sea Scrolls to the Forbidden Book at the Center for the Arts
@@ -6320,9 +6311,9 @@
 2005/4/27–2005/6/1: Dead Sea Scrolls to the Bible in America at the 
 2009/8/28–2009/9/20: The Dead Sea Scrolls &amp; the Ancient World at the The Arts House</v>
       </c>
-      <c r="F156" s="48"/>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F156" s="47"/>
+    </row>
+    <row r="157" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
         <v>19</v>
       </c>
@@ -6336,14 +6327,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E157" s="56" t="str" cm="1">
+      <c r="E157" s="55" t="str" cm="1">
         <f t="array" ref="E157">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F157" s="48"/>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F157" s="47"/>
+    </row>
+    <row r="158" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>19</v>
       </c>
@@ -6357,14 +6348,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E158" s="56" t="str" cm="1">
+      <c r="E158" s="55" t="str" cm="1">
         <f t="array" ref="E158">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F158" s="48"/>
-    </row>
-    <row r="159" spans="1:6" ht="268" x14ac:dyDescent="0.2">
+      <c r="F158" s="47"/>
+    </row>
+    <row r="159" spans="1:6" ht="255.75" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>19</v>
       </c>
@@ -6378,7 +6369,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>16</v>
       </c>
-      <c r="E159" s="56" t="str" cm="1">
+      <c r="E159" s="55" t="str" cm="1">
         <f t="array" ref="E159">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2003/3/17–2003/3/23: The European Fine Art Fair at the MECC
@@ -6398,9 +6389,9 @@
 2022/11/7–2022/11/10: Exhibition at the Aguttes Auction House
 2022/11/14–2022/11/15: Exhibition at the Aguttes Auction House</v>
       </c>
-      <c r="F159" s="48"/>
-    </row>
-    <row r="160" spans="1:6" ht="252" x14ac:dyDescent="0.2">
+      <c r="F159" s="47"/>
+    </row>
+    <row r="160" spans="1:6" ht="280.5" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>19</v>
       </c>
@@ -6414,7 +6405,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>17</v>
       </c>
-      <c r="E160" s="56" t="str" cm="1">
+      <c r="E160" s="55" t="str" cm="1">
         <f t="array" ref="E160">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2003/3/17–2003/3/23: The European Fine Art Fair at the MECC
@@ -6435,9 +6426,9 @@
 2022/11/7–2022/11/10: Exhibition at the Aguttes Auction House
 2022/11/14–2022/11/15: Exhibition at the Aguttes Auction House</v>
       </c>
-      <c r="F160" s="48"/>
-    </row>
-    <row r="161" spans="1:6" ht="135" x14ac:dyDescent="0.2">
+      <c r="F160" s="47"/>
+    </row>
+    <row r="161" spans="1:6" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>19</v>
       </c>
@@ -6451,7 +6442,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>11</v>
       </c>
-      <c r="E161" s="56" t="str" cm="1">
+      <c r="E161" s="55" t="str" cm="1">
         <f t="array" ref="E161">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2004/5/28–2004/6/20: Dead Sea Scrolls to the Bible in America at the Monroeville Expomart
@@ -6466,9 +6457,9 @@
 2022/11/7–2022/11/10: Exhibition at the Aguttes Auction House
 2022/11/14–2022/11/15: Exhibition at the Aguttes Auction House</v>
       </c>
-      <c r="F161" s="48"/>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F161" s="47"/>
+    </row>
+    <row r="162" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>19</v>
       </c>
@@ -6482,14 +6473,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E162" s="56" t="str" cm="1">
+      <c r="E162" s="55" t="str" cm="1">
         <f t="array" ref="E162">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F162" s="48"/>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F162" s="47"/>
+    </row>
+    <row r="163" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>19</v>
       </c>
@@ -6503,14 +6494,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E163" s="56" t="str" cm="1">
+      <c r="E163" s="55" t="str" cm="1">
         <f t="array" ref="E163">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F163" s="48"/>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F163" s="47"/>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>19</v>
       </c>
@@ -6524,14 +6515,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E164" s="56" t="str" cm="1">
+      <c r="E164" s="55" t="str" cm="1">
         <f t="array" ref="E164">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F164" s="48"/>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F164" s="47"/>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>19</v>
       </c>
@@ -6545,14 +6536,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E165" s="56" t="str" cm="1">
+      <c r="E165" s="55" t="str" cm="1">
         <f t="array" ref="E165">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F165" s="48"/>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F165" s="47"/>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>19</v>
       </c>
@@ -6566,14 +6557,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E166" s="56" t="str" cm="1">
+      <c r="E166" s="55" t="str" cm="1">
         <f t="array" ref="E166">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F166" s="48"/>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F166" s="47"/>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>19</v>
       </c>
@@ -6587,14 +6578,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E167" s="56" t="str" cm="1">
+      <c r="E167" s="55" t="str" cm="1">
         <f t="array" ref="E167">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F167" s="48"/>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F167" s="47"/>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>19</v>
       </c>
@@ -6608,14 +6599,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E168" s="56" t="str" cm="1">
+      <c r="E168" s="55" t="str" cm="1">
         <f t="array" ref="E168">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F168" s="48"/>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F168" s="47"/>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>19</v>
       </c>
@@ -6629,14 +6620,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E169" s="56" t="str" cm="1">
+      <c r="E169" s="55" t="str" cm="1">
         <f t="array" ref="E169">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F169" s="48"/>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F169" s="47"/>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>19</v>
       </c>
@@ -6650,14 +6641,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E170" s="56" t="str" cm="1">
+      <c r="E170" s="55" t="str" cm="1">
         <f t="array" ref="E170">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F170" s="48"/>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F170" s="47"/>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>19</v>
       </c>
@@ -6671,14 +6662,14 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E171" s="56" t="str" cm="1">
+      <c r="E171" s="55" t="str" cm="1">
         <f t="array" ref="E171">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F171" s="48"/>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F171" s="47"/>
+    </row>
+    <row r="172" spans="1:6" ht="24" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>19</v>
       </c>
@@ -6692,18 +6683,18 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E172" s="56" t="str" cm="1">
+      <c r="E172" s="55" t="str" cm="1">
         <f t="array" ref="E172">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F172" s="48"/>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A173" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B173" s="27" t="s">
+      <c r="F172" s="47"/>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A173" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B173" s="26" t="s">
         <v>148</v>
       </c>
       <c r="C173" s="10"/>
@@ -6711,18 +6702,18 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>None</v>
       </c>
-      <c r="E173" s="57" t="str" cm="1">
+      <c r="E173" s="56" t="str" cm="1">
         <f t="array" ref="E173">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v/>
       </c>
-      <c r="F173" s="48"/>
-    </row>
-    <row r="174" spans="1:6" ht="54" x14ac:dyDescent="0.2">
-      <c r="A174" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B174" s="28" t="s">
+      <c r="F173" s="47"/>
+    </row>
+    <row r="174" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A174" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B174" s="27" t="s">
         <v>40</v>
       </c>
       <c r="C174" s="3" t="s">
@@ -6732,20 +6723,20 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E174" s="56" t="str" cm="1">
+      <c r="E174" s="55" t="str" cm="1">
         <f t="array" ref="E174">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2005/1/14–2005/3/27: Dead Sea Scrolls to the Bible in America at the Providence Place
 2005/4/27–2005/6/1: Dead Sea Scrolls to the Bible in America at the 
 2008/2/9–2008/8/10: Highlights from the Israel Antiquities Authority: The Dead Sea Scrolls and 5,000 Years of Treasures at the Fine Arts Museum</v>
       </c>
-      <c r="F174" s="48"/>
-    </row>
-    <row r="175" spans="1:6" ht="135" x14ac:dyDescent="0.2">
-      <c r="A175" s="26" t="s">
+      <c r="F174" s="47"/>
+    </row>
+    <row r="175" spans="1:6" ht="132" x14ac:dyDescent="0.25">
+      <c r="A175" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B175" s="28" t="s">
+      <c r="B175" s="27" t="s">
         <v>42</v>
       </c>
       <c r="C175" s="3"/>
@@ -6753,7 +6744,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>8</v>
       </c>
-      <c r="E175" s="56" t="str" cm="1">
+      <c r="E175" s="55" t="str" cm="1">
         <f t="array" ref="E175">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1952/12/9–1952/12/9: Exhibition at the Palestine Archaeological Museum
@@ -6765,13 +6756,13 @@
 2015/9/21–2015/9/29: Verbum Domini II at the Pennsylvania Convetion Center
 2016/11/2–2016/11/12: 2000 Years of Jewish Culture: An Exhibition of Books, Manuscripts, Art and Jewelry at the Shapero Rare Books</v>
       </c>
-      <c r="F175" s="48"/>
-    </row>
-    <row r="176" spans="1:6" ht="256.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="26" t="s">
+      <c r="F175" s="47"/>
+    </row>
+    <row r="176" spans="1:6" ht="256.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="B176" s="28" t="s">
+      <c r="B176" s="27" t="s">
         <v>171</v>
       </c>
       <c r="C176" s="3"/>
@@ -6779,7 +6770,7 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>5</v>
       </c>
-      <c r="E176" s="56" t="str" cm="1">
+      <c r="E176" s="55" t="str" cm="1">
         <f t="array" ref="E176">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1993/4/29–1993/8/1: Scrolls from the Dead Sea: The Ancient Library of Qumran and Modern Scholarship at the Library of Congress
@@ -6788,10 +6779,12 @@
 1997/9/1–1997/9/18: Ancient Scrolls from the Dead Sea at the Brigham Young University Museum of Art
 1999/5/7–1999/8/8: Die Schriftrollen vom Toten Meer at the Stiftsbibliotek</v>
       </c>
-      <c r="F176" s="48"/>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A177" s="24"/>
+      <c r="F176" s="47"/>
+    </row>
+    <row r="177" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A177" s="23" t="s">
+        <v>10</v>
+      </c>
       <c r="B177" s="22" t="s">
         <v>260</v>
       </c>
@@ -6800,17 +6793,19 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E177" s="56" t="str" cm="1">
+      <c r="E177" s="55" t="str" cm="1">
         <f t="array" ref="E177">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2003/3/14–2003/3/23: The European Fine Art Fair at the MECC
 2003/3/17–2003/3/23: The European Fine Art Fair at the MECC
 2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
-      <c r="F177" s="49"/>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A178" s="24"/>
+      <c r="F177" s="48"/>
+    </row>
+    <row r="178" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A178" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="B178" s="22" t="s">
         <v>261</v>
       </c>
@@ -6819,16 +6814,18 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E178" s="56" t="str" cm="1">
+      <c r="E178" s="55" t="str" cm="1">
         <f t="array" ref="E178">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1971/6/19–1971/9/5: An Exhibition on the Dead Sea Scrolls at the American Bible Society
 1975/4/13–1975/5/4: The Book and the Spade at the Wisconsin Center</v>
       </c>
-      <c r="F178" s="49"/>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A179" s="24"/>
+      <c r="F178" s="48"/>
+    </row>
+    <row r="179" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A179" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="B179" s="22" t="s">
         <v>262</v>
       </c>
@@ -6837,16 +6834,18 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E179" s="56" t="str" cm="1">
+      <c r="E179" s="55" t="str" cm="1">
         <f t="array" ref="E179">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2003/6/17–2003/11/2: Archaeology and the Bible—From King David to the Dead Sea Scrolls at the Pointe-à-Callière
 2003/12/5–2004/4/12: Ancient Treasures and the Dead Sea Scrolls at the Canadian Museum of Civilization</v>
       </c>
-      <c r="F179" s="49"/>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A180" s="24"/>
+      <c r="F179" s="48"/>
+    </row>
+    <row r="180" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A180" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="B180" s="22" t="s">
         <v>263</v>
       </c>
@@ -6855,16 +6854,18 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E180" s="56" t="str" cm="1">
+      <c r="E180" s="55" t="str" cm="1">
         <f t="array" ref="E180">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1971/6/19–1971/9/5: An Exhibition on the Dead Sea Scrolls at the American Bible Society
 1975/4/13–1975/5/4: The Book and the Spade at the Wisconsin Center</v>
       </c>
-      <c r="F180" s="49"/>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A181" s="24"/>
+      <c r="F180" s="48"/>
+    </row>
+    <row r="181" spans="1:6" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A181" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="B181" s="22" t="s">
         <v>264</v>
       </c>
@@ -6873,16 +6874,18 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E181" s="56" t="str" cm="1">
+      <c r="E181" s="55" t="str" cm="1">
         <f t="array" ref="E181">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1971/6/19–1971/9/5: An Exhibition on the Dead Sea Scrolls at the American Bible Society
 1975/4/13–1975/5/4: The Book and the Spade at the Wisconsin Center</v>
       </c>
-      <c r="F181" s="49"/>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A182" s="24"/>
+      <c r="F181" s="48"/>
+    </row>
+    <row r="182" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A182" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="B182" s="22" t="s">
         <v>265</v>
       </c>
@@ -6891,15 +6894,17 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E182" s="56" t="str" cm="1">
+      <c r="E182" s="55" t="str" cm="1">
         <f t="array" ref="E182">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1998/7/29–1998/8/7: Congress of the International Organization for the study of the Old Testament at the University of Oslo</v>
       </c>
-      <c r="F182" s="49"/>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A183" s="23"/>
+      <c r="F182" s="48"/>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A183" s="23" t="s">
+        <v>2</v>
+      </c>
       <c r="B183" s="21" t="s">
         <v>266</v>
       </c>
@@ -6908,312 +6913,350 @@
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E183" s="57" t="str" cm="1">
+      <c r="E183" s="56" t="str" cm="1">
         <f t="array" ref="E183">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1951/1/1–2009/1/1: Exhibition at the Jordan Archaeological Museum</v>
       </c>
-      <c r="F183" s="49"/>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A184" s="59"/>
-      <c r="B184" s="60" t="s">
+      <c r="F183" s="48"/>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A184" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B184" s="58" t="s">
         <v>267</v>
       </c>
       <c r="C184" s="3"/>
-      <c r="D184" s="61">
+      <c r="D184" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E184" s="62" t="str" cm="1">
+      <c r="E184" s="55" t="str" cm="1">
         <f t="array" ref="E184">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A185" s="59"/>
-      <c r="B185" s="60" t="s">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A185" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B185" s="58" t="s">
         <v>268</v>
       </c>
       <c r="C185" s="3"/>
-      <c r="D185" s="61">
+      <c r="D185" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E185" s="62" t="str" cm="1">
+      <c r="E185" s="55" t="str" cm="1">
         <f t="array" ref="E185">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A186" s="59"/>
-      <c r="B186" s="60" t="s">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A186" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B186" s="58" t="s">
         <v>269</v>
       </c>
       <c r="C186" s="3"/>
-      <c r="D186" s="61">
+      <c r="D186" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E186" s="62" t="str" cm="1">
+      <c r="E186" s="55" t="str" cm="1">
         <f t="array" ref="E186">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A187" s="59"/>
-      <c r="B187" s="60" t="s">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A187" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B187" s="58" t="s">
         <v>270</v>
       </c>
       <c r="C187" s="3"/>
-      <c r="D187" s="61">
+      <c r="D187" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E187" s="62" t="str" cm="1">
+      <c r="E187" s="55" t="str" cm="1">
         <f t="array" ref="E187">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A188" s="59"/>
-      <c r="B188" s="60" t="s">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A188" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B188" s="58" t="s">
         <v>271</v>
       </c>
       <c r="C188" s="3"/>
-      <c r="D188" s="61">
+      <c r="D188" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E188" s="62" t="str" cm="1">
+      <c r="E188" s="55" t="str" cm="1">
         <f t="array" ref="E188">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A189" s="59"/>
-      <c r="B189" s="60" t="s">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A189" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B189" s="58" t="s">
         <v>272</v>
       </c>
       <c r="C189" s="3"/>
-      <c r="D189" s="61">
+      <c r="D189" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E189" s="62" t="str" cm="1">
+      <c r="E189" s="55" t="str" cm="1">
         <f t="array" ref="E189">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A190" s="59"/>
-      <c r="B190" s="60" t="s">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B190" s="58" t="s">
         <v>273</v>
       </c>
       <c r="C190" s="3"/>
-      <c r="D190" s="61">
+      <c r="D190" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E190" s="62" t="str" cm="1">
+      <c r="E190" s="55" t="str" cm="1">
         <f t="array" ref="E190">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A191" s="59"/>
-      <c r="B191" s="60" t="s">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B191" s="58" t="s">
         <v>274</v>
       </c>
       <c r="C191" s="3"/>
-      <c r="D191" s="61">
+      <c r="D191" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E191" s="62" t="str" cm="1">
+      <c r="E191" s="55" t="str" cm="1">
         <f t="array" ref="E191">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A192" s="59"/>
-      <c r="B192" s="60" t="s">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B192" s="58" t="s">
         <v>275</v>
       </c>
       <c r="C192" s="3"/>
-      <c r="D192" s="61">
+      <c r="D192" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E192" s="62" t="str" cm="1">
+      <c r="E192" s="55" t="str" cm="1">
         <f t="array" ref="E192">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A193" s="59"/>
-      <c r="B193" s="60" t="s">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B193" s="58" t="s">
         <v>276</v>
       </c>
       <c r="C193" s="3"/>
-      <c r="D193" s="61">
+      <c r="D193" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E193" s="62" t="str" cm="1">
+      <c r="E193" s="55" t="str" cm="1">
         <f t="array" ref="E193">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A194" s="59"/>
-      <c r="B194" s="60" t="s">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B194" s="58" t="s">
         <v>277</v>
       </c>
       <c r="C194" s="3"/>
-      <c r="D194" s="61">
+      <c r="D194" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E194" s="62" t="str" cm="1">
+      <c r="E194" s="55" t="str" cm="1">
         <f t="array" ref="E194">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A195" s="59"/>
-      <c r="B195" s="60" t="s">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B195" s="58" t="s">
         <v>278</v>
       </c>
       <c r="C195" s="3"/>
-      <c r="D195" s="61">
+      <c r="D195" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E195" s="62" t="str" cm="1">
+      <c r="E195" s="55" t="str" cm="1">
         <f t="array" ref="E195">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A196" s="59"/>
-      <c r="B196" s="60" t="s">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B196" s="58" t="s">
         <v>279</v>
       </c>
       <c r="C196" s="3"/>
-      <c r="D196" s="61">
+      <c r="D196" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E196" s="62" t="str" cm="1">
+      <c r="E196" s="55" t="str" cm="1">
         <f t="array" ref="E196">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A197" s="59"/>
-      <c r="B197" s="60" t="s">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B197" s="58" t="s">
         <v>280</v>
       </c>
       <c r="C197" s="3"/>
-      <c r="D197" s="61">
+      <c r="D197" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E197" s="62" t="str" cm="1">
+      <c r="E197" s="55" t="str" cm="1">
         <f t="array" ref="E197">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A198" s="59"/>
-      <c r="B198" s="60" t="s">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B198" s="58" t="s">
         <v>281</v>
       </c>
       <c r="C198" s="3"/>
-      <c r="D198" s="61">
+      <c r="D198" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E198" s="62" t="str" cm="1">
+      <c r="E198" s="55" t="str" cm="1">
         <f t="array" ref="E198">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A199" s="59"/>
-      <c r="B199" s="60" t="s">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B199" s="58" t="s">
         <v>282</v>
       </c>
       <c r="C199" s="3"/>
-      <c r="D199" s="61">
+      <c r="D199" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E199" s="62" t="str" cm="1">
+      <c r="E199" s="55" t="str" cm="1">
         <f t="array" ref="E199">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A200" s="59"/>
-      <c r="B200" s="60" t="s">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B200" s="58" t="s">
         <v>283</v>
       </c>
       <c r="C200" s="3"/>
-      <c r="D200" s="61">
+      <c r="D200" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E200" s="62" t="str" cm="1">
+      <c r="E200" s="55" t="str" cm="1">
         <f t="array" ref="E200">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A201" s="59"/>
-      <c r="B201" s="60" t="s">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="B201" s="58" t="s">
         <v>284</v>
       </c>
       <c r="C201" s="3"/>
-      <c r="D201" s="61">
+      <c r="D201" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E201" s="62" t="str" cm="1">
+      <c r="E201" s="55" t="str" cm="1">
         <f t="array" ref="E201">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2000/3/10–2000/6/18: The Dead Sea Scrolls at the Field Museum</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A202" s="59"/>
-      <c r="B202" s="60" t="s">
+    <row r="202" spans="1:5" ht="123.75" x14ac:dyDescent="0.25">
+      <c r="A202" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B202" s="58" t="s">
         <v>285</v>
       </c>
       <c r="C202" s="3"/>
-      <c r="D202" s="61">
+      <c r="D202" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>8</v>
       </c>
-      <c r="E202" s="62" t="str" cm="1">
+      <c r="E202" s="55" t="str" cm="1">
         <f t="array" ref="E202">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2005/2/5–2005/5/1: Ink &amp; Blood: Dead Sea Scrolls to the English Bible at the Knoxville Convention Center
@@ -7226,49 +7269,55 @@
 2012/2/3–2012/9/9: Ink &amp; Blood: Dead Sea Scrolls to Gutenberg at the Muzeo Museum and Cultural Center</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A203" s="59"/>
-      <c r="B203" s="60" t="s">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B203" s="58" t="s">
         <v>286</v>
       </c>
       <c r="C203" s="3"/>
-      <c r="D203" s="61">
+      <c r="D203" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E203" s="62" t="str" cm="1">
+      <c r="E203" s="55" t="str" cm="1">
         <f t="array" ref="E203">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2003/3/17–2003/3/23: The European Fine Art Fair at the MECC</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A204" s="59"/>
-      <c r="B204" s="60" t="s">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B204" s="58" t="s">
         <v>287</v>
       </c>
       <c r="C204" s="3"/>
-      <c r="D204" s="61">
+      <c r="D204" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E204" s="62" t="str" cm="1">
+      <c r="E204" s="55" t="str" cm="1">
         <f t="array" ref="E204">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2004/3/16–2004/4/18: From the Dead Sea Scrolls to the Forbidden Book at the John S. Knight Center</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A205" s="59"/>
-      <c r="B205" s="60" t="s">
+    <row r="205" spans="1:5" ht="66" x14ac:dyDescent="0.25">
+      <c r="A205" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B205" s="58" t="s">
         <v>288</v>
       </c>
       <c r="C205" s="3"/>
-      <c r="D205" s="61">
+      <c r="D205" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>4</v>
       </c>
-      <c r="E205" s="62" t="str" cm="1">
+      <c r="E205" s="55" t="str" cm="1">
         <f t="array" ref="E205">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2003/4/6–2003/4/29: From the Dead Sea Scrolls to the Forbidden Book at the Center for the Arts
@@ -7277,50 +7326,56 @@
 2004/1/5–2004/1/30: From the Dead Sea Scrolls to the Forbidden Book at the Von Braun Civic Center</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A206" s="59"/>
-      <c r="B206" s="60" t="s">
+    <row r="206" spans="1:5" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A206" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B206" s="58" t="s">
         <v>289</v>
       </c>
       <c r="C206" s="3"/>
-      <c r="D206" s="61">
+      <c r="D206" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>2</v>
       </c>
-      <c r="E206" s="62" t="str" cm="1">
+      <c r="E206" s="55" t="str" cm="1">
         <f t="array" ref="E206">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2003/3/17–2003/3/23: The European Fine Art Fair at the MECC
 2003/6/28–2003/6/28: Promotion of 'From the Dead Sea Scrolls to the Forbidden Book' at the South Fork Ranch</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A207" s="59"/>
-      <c r="B207" s="60" t="s">
+    <row r="207" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A207" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="B207" s="58" t="s">
         <v>290</v>
       </c>
       <c r="C207" s="3"/>
-      <c r="D207" s="61">
+      <c r="D207" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E207" s="62" t="str" cm="1">
+      <c r="E207" s="55" t="str" cm="1">
         <f t="array" ref="E207">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2012/7/2–2013/1/13: Dead Sea Scrolls &amp; the Bible: Ancient Artefacts, Timeless Treasures at the Southwestern Baptist Theological Seminary</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A208" s="59"/>
-      <c r="B208" s="60" t="s">
+    <row r="208" spans="1:5" ht="41.25" x14ac:dyDescent="0.25">
+      <c r="A208" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B208" s="58" t="s">
         <v>291</v>
       </c>
       <c r="C208" s="3"/>
-      <c r="D208" s="61">
+      <c r="D208" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>3</v>
       </c>
-      <c r="E208" s="62" t="str" cm="1">
+      <c r="E208" s="55" t="str" cm="1">
         <f t="array" ref="E208">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2007/6/20–2007/6/22: Dead Sea Scrolls and Ancient Material at the Church of Acts
@@ -7328,49 +7383,55 @@
 2007/10/7–2007/10/15: Dead Sea Scrolls and Ancient Material at the Suncoast Cathedral</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A209" s="59"/>
-      <c r="B209" s="60" t="s">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B209" s="58" t="s">
         <v>292</v>
       </c>
       <c r="C209" s="3"/>
-      <c r="D209" s="61">
+      <c r="D209" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E209" s="62" t="str" cm="1">
+      <c r="E209" s="55" t="str" cm="1">
         <f t="array" ref="E209">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>2005/5/21–1900/1/0: The New Hebrew: A Century of Art in Israel at the Martin Gropius-Bau Museum</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A210" s="59"/>
-      <c r="B210" s="60" t="s">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="23" t="s">
+        <v>297</v>
+      </c>
+      <c r="B210" s="58" t="s">
         <v>293</v>
       </c>
       <c r="C210" s="3"/>
-      <c r="D210" s="61">
+      <c r="D210" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E210" s="62" t="str" cm="1">
+      <c r="E210" s="55" t="str" cm="1">
         <f t="array" ref="E210">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v xml:space="preserve">1948/12/28–1948/12/30: The Fifth Convention of the Jewish Palestine Exploration Society at the </v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A211" s="59"/>
-      <c r="B211" s="60" t="s">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="B211" s="58" t="s">
         <v>294</v>
       </c>
       <c r="C211" s="3"/>
-      <c r="D211" s="61">
+      <c r="D211" s="42">
         <f>IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",IF(COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*")=0,"None",COUNTIF([1]!DDSExhibitions[Dead Sea Scrolls Exhibited],"*"&amp;DSSExhibited[[#This Row],[Manuscript]]&amp;"*"))),"None")</f>
         <v>1</v>
       </c>
-      <c r="E211" s="62" t="str" cm="1">
+      <c r="E211" s="55" t="str" cm="1">
         <f t="array" ref="E211">IFERROR(IF(DSSExhibited[[#This Row],[Manuscript]]="","",_xlfn.TEXTJOIN("
 ",TRUE,_xlfn._xlws.FILTER([1]!DDSExhibitions[Summarising],ISNUMBER(SEARCH(DSSExhibited[[#This Row],[Manuscript]],[1]!DDSExhibitions[Dead Sea Scrolls Exhibited]))))),"")</f>
         <v>1968/5/8–1968/9/2: Israel through the Ages at the Petit Palais</v>

</xml_diff>